<commit_message>
hardware: boms: Updating bill of materials with new template in the outputs and fabrication folders
</commit_message>
<xml_diff>
--- a/hardware/fabrication/board_bom.xlsx
+++ b/hardware/fabrication/board_bom.xlsx
@@ -1,11 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23628"/>
   <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6FE72850-D37A-4B72-B4E1-A056D1AA981F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Yan Azeredo\Desktop\SpaceLab\eps2\hardware\fabrication\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABED8592-ACEA-40A9-AFAA-A254B76C60BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2655" yWindow="1890" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -33,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="344">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="345">
   <si>
     <t>Source Data From:</t>
   </si>
@@ -1065,6 +1070,9 @@
   </si>
   <si>
     <t>Fitted</t>
+  </si>
+  <si>
+    <t>RC0805FR-071KL</t>
   </si>
 </sst>
 </file>
@@ -1287,6 +1295,15 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1296,20 +1313,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2233,8 +2241,8 @@
   </sheetPr>
   <dimension ref="A1:M114"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView tabSelected="1" view="pageBreakPreview" topLeftCell="A34" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
+      <selection activeCell="F43" sqref="F43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2257,11 +2265,11 @@
       <c r="A1" s="1"/>
       <c r="B1" s="17"/>
       <c r="C1" s="17"/>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E1" s="25"/>
-      <c r="F1" s="26"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="29"/>
       <c r="G1" s="18"/>
       <c r="H1" s="18"/>
       <c r="I1" s="18"/>
@@ -2277,10 +2285,10 @@
       <c r="D2" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="E2" s="28" t="s">
+      <c r="E2" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F2" s="27"/>
+      <c r="F2" s="31"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
       <c r="I2" s="20"/>
@@ -2296,10 +2304,10 @@
       <c r="D3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="E3" s="28" t="s">
+      <c r="E3" s="30" t="s">
         <v>8</v>
       </c>
-      <c r="F3" s="27"/>
+      <c r="F3" s="31"/>
       <c r="G3" s="20"/>
       <c r="H3" s="20"/>
       <c r="I3" s="20"/>
@@ -2315,10 +2323,10 @@
       <c r="D4" s="21" t="s">
         <v>2</v>
       </c>
-      <c r="E4" s="28" t="s">
+      <c r="E4" s="30" t="s">
         <v>9</v>
       </c>
-      <c r="F4" s="27"/>
+      <c r="F4" s="31"/>
       <c r="G4" s="19"/>
       <c r="H4" s="20"/>
       <c r="I4" s="20"/>
@@ -2334,10 +2342,10 @@
       <c r="D5" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="E5" s="28" t="s">
+      <c r="E5" s="30" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="27"/>
+      <c r="F5" s="31"/>
       <c r="G5" s="20"/>
       <c r="H5" s="20"/>
       <c r="I5" s="20"/>
@@ -2353,10 +2361,10 @@
       <c r="D6" s="22" t="s">
         <v>3</v>
       </c>
-      <c r="E6" s="29" t="s">
+      <c r="E6" s="24" t="s">
         <v>11</v>
       </c>
-      <c r="F6" s="29" t="s">
+      <c r="F6" s="24" t="s">
         <v>12</v>
       </c>
       <c r="G6" s="20"/>
@@ -2376,11 +2384,11 @@
       </c>
       <c r="E7" s="7">
         <f ca="1">TODAY()</f>
-        <v>44229</v>
+        <v>44252</v>
       </c>
       <c r="F7" s="8">
         <f ca="1">NOW()</f>
-        <v>44229.060284259256</v>
+        <v>44252.99559849537</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="20"/>
@@ -2461,32 +2469,32 @@
         <f>ROW(A11) - ROW($A$10)</f>
         <v>1</v>
       </c>
-      <c r="B11" s="30" t="s">
+      <c r="B11" s="25" t="s">
         <v>14</v>
       </c>
       <c r="C11" s="14">
         <v>44</v>
       </c>
-      <c r="D11" s="30" t="s">
+      <c r="D11" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="E11" s="30" t="s">
+      <c r="E11" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="F11" s="30" t="s">
+      <c r="F11" s="25" t="s">
         <v>134</v>
       </c>
-      <c r="G11" s="31" t="s">
+      <c r="G11" s="26" t="s">
         <v>225</v>
       </c>
       <c r="H11" s="15"/>
-      <c r="I11" s="31" t="s">
+      <c r="I11" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="J11" s="31" t="s">
+      <c r="J11" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K11" s="31" t="s">
+      <c r="K11" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2495,32 +2503,32 @@
         <f t="shared" ref="A12:A94" si="0">ROW(A12) - ROW($A$10)</f>
         <v>2</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="25" t="s">
         <v>15</v>
       </c>
       <c r="C12" s="14">
         <v>19</v>
       </c>
-      <c r="D12" s="30" t="s">
+      <c r="D12" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="E12" s="30" t="s">
+      <c r="E12" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="F12" s="30" t="s">
+      <c r="F12" s="25" t="s">
         <v>135</v>
       </c>
-      <c r="G12" s="31" t="s">
+      <c r="G12" s="26" t="s">
         <v>226</v>
       </c>
       <c r="H12" s="15"/>
-      <c r="I12" s="31" t="s">
+      <c r="I12" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="J12" s="31" t="s">
+      <c r="J12" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K12" s="31" t="s">
+      <c r="K12" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2529,32 +2537,32 @@
         <f>ROW(A13) - ROW($A$10)</f>
         <v>3</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="25" t="s">
         <v>16</v>
       </c>
       <c r="C13" s="14">
         <v>15</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="E13" s="30" t="s">
+      <c r="E13" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="F13" s="30" t="s">
+      <c r="F13" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="G13" s="31" t="s">
+      <c r="G13" s="26" t="s">
         <v>227</v>
       </c>
       <c r="H13" s="15"/>
-      <c r="I13" s="31" t="s">
+      <c r="I13" s="26" t="s">
         <v>306</v>
       </c>
-      <c r="J13" s="31" t="s">
+      <c r="J13" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K13" s="31" t="s">
+      <c r="K13" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2563,32 +2571,32 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="25" t="s">
         <v>17</v>
       </c>
       <c r="C14" s="14">
         <v>14</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="25" t="s">
         <v>137</v>
       </c>
-      <c r="G14" s="31" t="s">
+      <c r="G14" s="26" t="s">
         <v>228</v>
       </c>
       <c r="H14" s="15"/>
-      <c r="I14" s="31" t="s">
+      <c r="I14" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J14" s="31" t="s">
+      <c r="J14" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K14" s="31" t="s">
+      <c r="K14" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2597,32 +2605,32 @@
         <f>ROW(A15) - ROW($A$10)</f>
         <v>5</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="25" t="s">
         <v>18</v>
       </c>
       <c r="C15" s="14">
         <v>12</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="F15" s="30" t="s">
+      <c r="F15" s="25" t="s">
         <v>138</v>
       </c>
-      <c r="G15" s="31" t="s">
+      <c r="G15" s="26" t="s">
         <v>229</v>
       </c>
       <c r="H15" s="15"/>
-      <c r="I15" s="31" t="s">
+      <c r="I15" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J15" s="31" t="s">
+      <c r="J15" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K15" s="31" t="s">
+      <c r="K15" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2631,32 +2639,32 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="25" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="14">
         <v>11</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="E16" s="30" t="s">
+      <c r="E16" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="F16" s="30" t="s">
+      <c r="F16" s="25" t="s">
         <v>139</v>
       </c>
-      <c r="G16" s="31" t="s">
+      <c r="G16" s="26" t="s">
         <v>230</v>
       </c>
       <c r="H16" s="15"/>
-      <c r="I16" s="31" t="s">
+      <c r="I16" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="J16" s="31" t="s">
+      <c r="J16" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K16" s="31" t="s">
+      <c r="K16" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2665,32 +2673,32 @@
         <f>ROW(A17) - ROW($A$10)</f>
         <v>7</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="25" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="14">
         <v>10</v>
       </c>
-      <c r="D17" s="30" t="s">
+      <c r="D17" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="E17" s="30" t="s">
+      <c r="E17" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="F17" s="30" t="s">
+      <c r="F17" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="G17" s="31" t="s">
+      <c r="G17" s="26" t="s">
         <v>231</v>
       </c>
       <c r="H17" s="15"/>
-      <c r="I17" s="31" t="s">
+      <c r="I17" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="J17" s="31" t="s">
+      <c r="J17" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K17" s="31" t="s">
+      <c r="K17" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2699,32 +2707,32 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="25" t="s">
         <v>21</v>
       </c>
       <c r="C18" s="14">
         <v>9</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="E18" s="30" t="s">
+      <c r="E18" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="F18" s="30" t="s">
+      <c r="F18" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="G18" s="31" t="s">
+      <c r="G18" s="26" t="s">
         <v>232</v>
       </c>
       <c r="H18" s="15"/>
-      <c r="I18" s="31" t="s">
+      <c r="I18" s="26" t="s">
         <v>310</v>
       </c>
-      <c r="J18" s="31" t="s">
+      <c r="J18" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K18" s="31" t="s">
+      <c r="K18" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2733,32 +2741,32 @@
         <f>ROW(A19) - ROW($A$10)</f>
         <v>9</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="25" t="s">
         <v>22</v>
       </c>
       <c r="C19" s="14">
         <v>8</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="F19" s="30" t="s">
+      <c r="F19" s="25" t="s">
         <v>142</v>
       </c>
-      <c r="G19" s="31" t="s">
+      <c r="G19" s="26" t="s">
         <v>233</v>
       </c>
       <c r="H19" s="15"/>
-      <c r="I19" s="31" t="s">
+      <c r="I19" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="J19" s="31" t="s">
+      <c r="J19" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K19" s="31" t="s">
+      <c r="K19" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2767,32 +2775,32 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B20" s="30" t="s">
+      <c r="B20" s="25" t="s">
         <v>23</v>
       </c>
       <c r="C20" s="14">
         <v>8</v>
       </c>
-      <c r="D20" s="30" t="s">
+      <c r="D20" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="E20" s="30" t="s">
+      <c r="E20" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="F20" s="30" t="s">
+      <c r="F20" s="25" t="s">
         <v>143</v>
       </c>
-      <c r="G20" s="31" t="s">
+      <c r="G20" s="26" t="s">
         <v>234</v>
       </c>
       <c r="H20" s="15"/>
-      <c r="I20" s="31" t="s">
+      <c r="I20" s="26" t="s">
         <v>312</v>
       </c>
-      <c r="J20" s="31" t="s">
+      <c r="J20" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K20" s="31" t="s">
+      <c r="K20" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2801,32 +2809,32 @@
         <f>ROW(A21) - ROW($A$10)</f>
         <v>11</v>
       </c>
-      <c r="B21" s="30" t="s">
+      <c r="B21" s="25" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="14">
         <v>7</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="E21" s="30" t="s">
+      <c r="E21" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="F21" s="30" t="s">
+      <c r="F21" s="25" t="s">
         <v>144</v>
       </c>
-      <c r="G21" s="31" t="s">
+      <c r="G21" s="26" t="s">
         <v>235</v>
       </c>
       <c r="H21" s="15"/>
-      <c r="I21" s="31" t="s">
+      <c r="I21" s="26" t="s">
         <v>313</v>
       </c>
-      <c r="J21" s="31" t="s">
+      <c r="J21" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K21" s="31" t="s">
+      <c r="K21" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2835,32 +2843,32 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B22" s="30" t="s">
+      <c r="B22" s="25" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="14">
         <v>7</v>
       </c>
-      <c r="D22" s="30" t="s">
+      <c r="D22" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="E22" s="30" t="s">
+      <c r="E22" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="F22" s="30" t="s">
+      <c r="F22" s="25" t="s">
         <v>145</v>
       </c>
-      <c r="G22" s="31" t="s">
+      <c r="G22" s="26" t="s">
         <v>236</v>
       </c>
       <c r="H22" s="15"/>
-      <c r="I22" s="31" t="s">
+      <c r="I22" s="26" t="s">
         <v>314</v>
       </c>
-      <c r="J22" s="31" t="s">
+      <c r="J22" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K22" s="31" t="s">
+      <c r="K22" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2869,32 +2877,32 @@
         <f>ROW(A23) - ROW($A$10)</f>
         <v>13</v>
       </c>
-      <c r="B23" s="30" t="s">
+      <c r="B23" s="25" t="s">
         <v>26</v>
       </c>
       <c r="C23" s="14">
         <v>7</v>
       </c>
-      <c r="D23" s="30" t="s">
+      <c r="D23" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="E23" s="30" t="s">
+      <c r="E23" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="F23" s="30" t="s">
+      <c r="F23" s="25" t="s">
         <v>146</v>
       </c>
-      <c r="G23" s="31" t="s">
+      <c r="G23" s="26" t="s">
         <v>146</v>
       </c>
       <c r="H23" s="15"/>
-      <c r="I23" s="31" t="s">
+      <c r="I23" s="26" t="s">
         <v>315</v>
       </c>
-      <c r="J23" s="31" t="s">
+      <c r="J23" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K23" s="31" t="s">
+      <c r="K23" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2903,32 +2911,32 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B24" s="30" t="s">
+      <c r="B24" s="25" t="s">
         <v>27</v>
       </c>
       <c r="C24" s="14">
         <v>6</v>
       </c>
-      <c r="D24" s="30" t="s">
+      <c r="D24" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="E24" s="30" t="s">
+      <c r="E24" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="F24" s="30" t="s">
+      <c r="F24" s="25" t="s">
         <v>147</v>
       </c>
-      <c r="G24" s="31" t="s">
+      <c r="G24" s="26" t="s">
         <v>237</v>
       </c>
       <c r="H24" s="15"/>
-      <c r="I24" s="31" t="s">
+      <c r="I24" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="J24" s="31" t="s">
+      <c r="J24" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K24" s="31" t="s">
+      <c r="K24" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2937,32 +2945,32 @@
         <f>ROW(A25) - ROW($A$10)</f>
         <v>15</v>
       </c>
-      <c r="B25" s="30" t="s">
+      <c r="B25" s="25" t="s">
         <v>28</v>
       </c>
       <c r="C25" s="14">
         <v>6</v>
       </c>
-      <c r="D25" s="30" t="s">
+      <c r="D25" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E25" s="30" t="s">
+      <c r="E25" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="F25" s="30" t="s">
+      <c r="F25" s="25" t="s">
         <v>148</v>
       </c>
-      <c r="G25" s="31" t="s">
+      <c r="G25" s="26" t="s">
         <v>238</v>
       </c>
       <c r="H25" s="15"/>
-      <c r="I25" s="31" t="s">
+      <c r="I25" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="J25" s="31" t="s">
+      <c r="J25" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K25" s="31" t="s">
+      <c r="K25" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -2971,32 +2979,32 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B26" s="30" t="s">
+      <c r="B26" s="25" t="s">
         <v>29</v>
       </c>
       <c r="C26" s="14">
         <v>6</v>
       </c>
-      <c r="D26" s="30" t="s">
+      <c r="D26" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E26" s="30" t="s">
+      <c r="E26" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="F26" s="30" t="s">
+      <c r="F26" s="25" t="s">
         <v>149</v>
       </c>
-      <c r="G26" s="31" t="s">
+      <c r="G26" s="26" t="s">
         <v>239</v>
       </c>
       <c r="H26" s="15"/>
-      <c r="I26" s="31" t="s">
+      <c r="I26" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J26" s="31" t="s">
+      <c r="J26" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K26" s="31" t="s">
+      <c r="K26" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3005,32 +3013,32 @@
         <f>ROW(A27) - ROW($A$10)</f>
         <v>17</v>
       </c>
-      <c r="B27" s="30" t="s">
+      <c r="B27" s="25" t="s">
         <v>30</v>
       </c>
       <c r="C27" s="14">
         <v>5</v>
       </c>
-      <c r="D27" s="30" t="s">
+      <c r="D27" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E27" s="30" t="s">
+      <c r="E27" s="25" t="s">
         <v>150</v>
       </c>
-      <c r="F27" s="30" t="s">
+      <c r="F27" s="25" t="s">
         <v>218</v>
       </c>
-      <c r="G27" s="31" t="s">
+      <c r="G27" s="26" t="s">
         <v>240</v>
       </c>
       <c r="H27" s="15"/>
-      <c r="I27" s="31" t="s">
+      <c r="I27" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J27" s="31" t="s">
+      <c r="J27" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K27" s="31" t="s">
+      <c r="K27" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3039,32 +3047,32 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B28" s="30" t="s">
+      <c r="B28" s="25" t="s">
         <v>31</v>
       </c>
       <c r="C28" s="14">
         <v>5</v>
       </c>
-      <c r="D28" s="30" t="s">
+      <c r="D28" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="E28" s="30" t="s">
+      <c r="E28" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="F28" s="30" t="s">
+      <c r="F28" s="25" t="s">
         <v>151</v>
       </c>
-      <c r="G28" s="31" t="s">
+      <c r="G28" s="26" t="s">
         <v>241</v>
       </c>
       <c r="H28" s="15"/>
-      <c r="I28" s="31" t="s">
+      <c r="I28" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="J28" s="31" t="s">
+      <c r="J28" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K28" s="31" t="s">
+      <c r="K28" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3073,32 +3081,32 @@
         <f>ROW(A29) - ROW($A$10)</f>
         <v>19</v>
       </c>
-      <c r="B29" s="30" t="s">
+      <c r="B29" s="25" t="s">
         <v>32</v>
       </c>
       <c r="C29" s="14">
         <v>5</v>
       </c>
-      <c r="D29" s="30" t="s">
+      <c r="D29" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="30" t="s">
+      <c r="E29" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="F29" s="30" t="s">
+      <c r="F29" s="25" t="s">
         <v>152</v>
       </c>
-      <c r="G29" s="31" t="s">
+      <c r="G29" s="26" t="s">
         <v>242</v>
       </c>
       <c r="H29" s="15"/>
-      <c r="I29" s="31" t="s">
+      <c r="I29" s="26" t="s">
         <v>318</v>
       </c>
-      <c r="J29" s="31" t="s">
+      <c r="J29" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K29" s="31" t="s">
+      <c r="K29" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3107,32 +3115,32 @@
         <f t="shared" si="0"/>
         <v>20</v>
       </c>
-      <c r="B30" s="30" t="s">
+      <c r="B30" s="25" t="s">
         <v>33</v>
       </c>
       <c r="C30" s="14">
         <v>5</v>
       </c>
-      <c r="D30" s="30" t="s">
+      <c r="D30" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E30" s="30" t="s">
+      <c r="E30" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="F30" s="30" t="s">
+      <c r="F30" s="25" t="s">
         <v>153</v>
       </c>
-      <c r="G30" s="31" t="s">
+      <c r="G30" s="26" t="s">
         <v>153</v>
       </c>
       <c r="H30" s="15"/>
-      <c r="I30" s="31" t="s">
+      <c r="I30" s="26" t="s">
         <v>319</v>
       </c>
-      <c r="J30" s="31" t="s">
+      <c r="J30" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K30" s="31" t="s">
+      <c r="K30" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3141,32 +3149,32 @@
         <f>ROW(A31) - ROW($A$10)</f>
         <v>21</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="25" t="s">
         <v>34</v>
       </c>
       <c r="C31" s="14">
         <v>4</v>
       </c>
-      <c r="D31" s="30" t="s">
+      <c r="D31" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="F31" s="30" t="s">
+      <c r="F31" s="25" t="s">
         <v>154</v>
       </c>
-      <c r="G31" s="31" t="s">
+      <c r="G31" s="26" t="s">
         <v>243</v>
       </c>
       <c r="H31" s="15"/>
-      <c r="I31" s="31" t="s">
+      <c r="I31" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J31" s="31" t="s">
+      <c r="J31" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K31" s="31" t="s">
+      <c r="K31" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3175,32 +3183,32 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B32" s="30" t="s">
+      <c r="B32" s="25" t="s">
         <v>35</v>
       </c>
       <c r="C32" s="14">
         <v>4</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="E32" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="F32" s="30" t="s">
+      <c r="F32" s="25" t="s">
         <v>155</v>
       </c>
-      <c r="G32" s="31" t="s">
+      <c r="G32" s="26" t="s">
         <v>244</v>
       </c>
       <c r="H32" s="15"/>
-      <c r="I32" s="31" t="s">
+      <c r="I32" s="26" t="s">
         <v>309</v>
       </c>
-      <c r="J32" s="31" t="s">
+      <c r="J32" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K32" s="31" t="s">
+      <c r="K32" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3209,32 +3217,32 @@
         <f>ROW(A33) - ROW($A$10)</f>
         <v>23</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="25" t="s">
         <v>36</v>
       </c>
       <c r="C33" s="14">
         <v>4</v>
       </c>
-      <c r="D33" s="30" t="s">
+      <c r="D33" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="E33" s="30" t="s">
+      <c r="E33" s="25" t="s">
         <v>114</v>
       </c>
-      <c r="F33" s="30" t="s">
+      <c r="F33" s="25" t="s">
         <v>219</v>
       </c>
-      <c r="G33" s="31" t="s">
+      <c r="G33" s="26" t="s">
         <v>245</v>
       </c>
       <c r="H33" s="15"/>
-      <c r="I33" s="31" t="s">
+      <c r="I33" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J33" s="31" t="s">
+      <c r="J33" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K33" s="31" t="s">
+      <c r="K33" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3243,32 +3251,32 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="25" t="s">
         <v>37</v>
       </c>
       <c r="C34" s="14">
         <v>4</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="E34" s="30" t="s">
+      <c r="E34" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="F34" s="30" t="s">
+      <c r="F34" s="25" t="s">
         <v>156</v>
       </c>
-      <c r="G34" s="31" t="s">
+      <c r="G34" s="26" t="s">
         <v>246</v>
       </c>
       <c r="H34" s="15"/>
-      <c r="I34" s="31" t="s">
+      <c r="I34" s="26" t="s">
         <v>320</v>
       </c>
-      <c r="J34" s="31" t="s">
+      <c r="J34" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K34" s="31" t="s">
+      <c r="K34" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3277,32 +3285,32 @@
         <f>ROW(A35) - ROW($A$10)</f>
         <v>25</v>
       </c>
-      <c r="B35" s="30" t="s">
+      <c r="B35" s="25" t="s">
         <v>38</v>
       </c>
       <c r="C35" s="14">
         <v>4</v>
       </c>
-      <c r="D35" s="30" t="s">
+      <c r="D35" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="E35" s="30" t="s">
+      <c r="E35" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="F35" s="30" t="s">
+      <c r="F35" s="25" t="s">
         <v>157</v>
       </c>
-      <c r="G35" s="31" t="s">
+      <c r="G35" s="26" t="s">
         <v>247</v>
       </c>
       <c r="H35" s="15"/>
-      <c r="I35" s="31" t="s">
+      <c r="I35" s="26" t="s">
         <v>318</v>
       </c>
-      <c r="J35" s="31" t="s">
+      <c r="J35" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K35" s="31" t="s">
+      <c r="K35" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3311,32 +3319,32 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B36" s="30" t="s">
+      <c r="B36" s="25" t="s">
         <v>39</v>
       </c>
       <c r="C36" s="14">
         <v>3</v>
       </c>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E36" s="30" t="s">
+      <c r="E36" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="F36" s="30" t="s">
+      <c r="F36" s="25" t="s">
         <v>220</v>
       </c>
-      <c r="G36" s="31" t="s">
+      <c r="G36" s="26" t="s">
         <v>248</v>
       </c>
       <c r="H36" s="15"/>
-      <c r="I36" s="31" t="s">
+      <c r="I36" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J36" s="31" t="s">
+      <c r="J36" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K36" s="31" t="s">
+      <c r="K36" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3345,32 +3353,32 @@
         <f>ROW(A37) - ROW($A$10)</f>
         <v>27</v>
       </c>
-      <c r="B37" s="30" t="s">
+      <c r="B37" s="25" t="s">
         <v>40</v>
       </c>
       <c r="C37" s="14">
         <v>3</v>
       </c>
-      <c r="D37" s="30" t="s">
+      <c r="D37" s="25" t="s">
         <v>116</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="E37" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="F37" s="30" t="s">
+      <c r="F37" s="25" t="s">
         <v>159</v>
       </c>
-      <c r="G37" s="31" t="s">
+      <c r="G37" s="26" t="s">
         <v>249</v>
       </c>
       <c r="H37" s="15"/>
-      <c r="I37" s="31" t="s">
+      <c r="I37" s="26" t="s">
         <v>321</v>
       </c>
-      <c r="J37" s="31" t="s">
+      <c r="J37" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K37" s="31" t="s">
+      <c r="K37" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3379,32 +3387,32 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="25" t="s">
         <v>41</v>
       </c>
       <c r="C38" s="14">
         <v>3</v>
       </c>
-      <c r="D38" s="30" t="s">
+      <c r="D38" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="F38" s="30" t="s">
+      <c r="F38" s="25" t="s">
         <v>160</v>
       </c>
-      <c r="G38" s="31" t="s">
+      <c r="G38" s="26" t="s">
         <v>250</v>
       </c>
       <c r="H38" s="15"/>
-      <c r="I38" s="31" t="s">
+      <c r="I38" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J38" s="31" t="s">
+      <c r="J38" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K38" s="31" t="s">
+      <c r="K38" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3413,32 +3421,32 @@
         <f>ROW(A39) - ROW($A$10)</f>
         <v>29</v>
       </c>
-      <c r="B39" s="30" t="s">
+      <c r="B39" s="25" t="s">
         <v>42</v>
       </c>
       <c r="C39" s="14">
         <v>3</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E39" s="30" t="s">
+      <c r="E39" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="F39" s="30" t="s">
+      <c r="F39" s="25" t="s">
         <v>161</v>
       </c>
-      <c r="G39" s="31" t="s">
+      <c r="G39" s="26" t="s">
         <v>251</v>
       </c>
       <c r="H39" s="15"/>
-      <c r="I39" s="31" t="s">
+      <c r="I39" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J39" s="31" t="s">
+      <c r="J39" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K39" s="31" t="s">
+      <c r="K39" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3447,32 +3455,32 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B40" s="30" t="s">
+      <c r="B40" s="25" t="s">
         <v>43</v>
       </c>
       <c r="C40" s="14">
         <v>3</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="E40" s="30" t="s">
+      <c r="E40" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="F40" s="30" t="s">
+      <c r="F40" s="25" t="s">
         <v>162</v>
       </c>
-      <c r="G40" s="31" t="s">
+      <c r="G40" s="26" t="s">
         <v>252</v>
       </c>
       <c r="H40" s="15"/>
-      <c r="I40" s="31" t="s">
+      <c r="I40" s="26" t="s">
         <v>322</v>
       </c>
-      <c r="J40" s="31" t="s">
+      <c r="J40" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K40" s="31" t="s">
+      <c r="K40" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3481,32 +3489,32 @@
         <f>ROW(A41) - ROW($A$10)</f>
         <v>31</v>
       </c>
-      <c r="B41" s="30" t="s">
+      <c r="B41" s="25" t="s">
         <v>44</v>
       </c>
       <c r="C41" s="14">
         <v>3</v>
       </c>
-      <c r="D41" s="30" t="s">
+      <c r="D41" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="E41" s="30" t="s">
+      <c r="E41" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="F41" s="30" t="s">
+      <c r="F41" s="25" t="s">
         <v>163</v>
       </c>
-      <c r="G41" s="31" t="s">
+      <c r="G41" s="26" t="s">
         <v>253</v>
       </c>
       <c r="H41" s="15"/>
-      <c r="I41" s="31" t="s">
+      <c r="I41" s="26" t="s">
         <v>323</v>
       </c>
-      <c r="J41" s="31" t="s">
+      <c r="J41" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K41" s="31" t="s">
+      <c r="K41" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3515,32 +3523,32 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B42" s="30" t="s">
+      <c r="B42" s="25" t="s">
         <v>45</v>
       </c>
       <c r="C42" s="14">
         <v>2</v>
       </c>
-      <c r="D42" s="30" t="s">
+      <c r="D42" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="E42" s="30" t="s">
+      <c r="E42" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="F42" s="30" t="s">
+      <c r="F42" s="25" t="s">
         <v>164</v>
       </c>
-      <c r="G42" s="31" t="s">
+      <c r="G42" s="26" t="s">
         <v>254</v>
       </c>
       <c r="H42" s="15"/>
-      <c r="I42" s="31" t="s">
+      <c r="I42" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="J42" s="31" t="s">
+      <c r="J42" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K42" s="31" t="s">
+      <c r="K42" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3549,32 +3557,32 @@
         <f>ROW(A43) - ROW($A$10)</f>
         <v>33</v>
       </c>
-      <c r="B43" s="30" t="s">
+      <c r="B43" s="25" t="s">
         <v>46</v>
       </c>
       <c r="C43" s="14">
         <v>2</v>
       </c>
-      <c r="D43" s="30" t="s">
+      <c r="D43" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="E43" s="30" t="s">
+      <c r="E43" s="25" t="s">
         <v>165</v>
       </c>
-      <c r="F43" s="30" t="s">
-        <v>114</v>
-      </c>
-      <c r="G43" s="31" t="s">
+      <c r="F43" s="25" t="s">
+        <v>344</v>
+      </c>
+      <c r="G43" s="26" t="s">
         <v>255</v>
       </c>
       <c r="H43" s="15"/>
-      <c r="I43" s="31" t="s">
+      <c r="I43" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J43" s="31" t="s">
+      <c r="J43" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K43" s="31" t="s">
+      <c r="K43" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3583,32 +3591,32 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B44" s="30" t="s">
+      <c r="B44" s="25" t="s">
         <v>47</v>
       </c>
       <c r="C44" s="14">
         <v>2</v>
       </c>
-      <c r="D44" s="30" t="s">
+      <c r="D44" s="25" t="s">
         <v>118</v>
       </c>
-      <c r="E44" s="30" t="s">
+      <c r="E44" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="F44" s="30" t="s">
+      <c r="F44" s="25" t="s">
         <v>166</v>
       </c>
-      <c r="G44" s="31" t="s">
+      <c r="G44" s="26" t="s">
         <v>256</v>
       </c>
       <c r="H44" s="15"/>
-      <c r="I44" s="31" t="s">
+      <c r="I44" s="26" t="s">
         <v>324</v>
       </c>
-      <c r="J44" s="31" t="s">
+      <c r="J44" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K44" s="31" t="s">
+      <c r="K44" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3617,32 +3625,32 @@
         <f>ROW(A45) - ROW($A$10)</f>
         <v>35</v>
       </c>
-      <c r="B45" s="30" t="s">
+      <c r="B45" s="25" t="s">
         <v>48</v>
       </c>
       <c r="C45" s="14">
         <v>2</v>
       </c>
-      <c r="D45" s="30" t="s">
+      <c r="D45" s="25" t="s">
         <v>119</v>
       </c>
-      <c r="E45" s="30" t="s">
+      <c r="E45" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="F45" s="30" t="s">
+      <c r="F45" s="25" t="s">
         <v>167</v>
       </c>
-      <c r="G45" s="31" t="s">
+      <c r="G45" s="26" t="s">
         <v>257</v>
       </c>
       <c r="H45" s="15"/>
-      <c r="I45" s="31" t="s">
+      <c r="I45" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="J45" s="31" t="s">
+      <c r="J45" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K45" s="31" t="s">
+      <c r="K45" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3651,32 +3659,32 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B46" s="30" t="s">
+      <c r="B46" s="25" t="s">
         <v>49</v>
       </c>
       <c r="C46" s="14">
         <v>2</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="E46" s="30" t="s">
+      <c r="E46" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="F46" s="30" t="s">
+      <c r="F46" s="25" t="s">
         <v>168</v>
       </c>
-      <c r="G46" s="31" t="s">
+      <c r="G46" s="26" t="s">
         <v>258</v>
       </c>
       <c r="H46" s="15"/>
-      <c r="I46" s="31" t="s">
+      <c r="I46" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J46" s="31" t="s">
+      <c r="J46" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K46" s="31" t="s">
+      <c r="K46" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3685,32 +3693,32 @@
         <f>ROW(A47) - ROW($A$10)</f>
         <v>37</v>
       </c>
-      <c r="B47" s="30" t="s">
+      <c r="B47" s="25" t="s">
         <v>50</v>
       </c>
       <c r="C47" s="14">
         <v>2</v>
       </c>
-      <c r="D47" s="30" t="s">
+      <c r="D47" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="E47" s="30" t="s">
+      <c r="E47" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="F47" s="30" t="s">
+      <c r="F47" s="25" t="s">
         <v>169</v>
       </c>
-      <c r="G47" s="31" t="s">
+      <c r="G47" s="26" t="s">
         <v>259</v>
       </c>
       <c r="H47" s="15"/>
-      <c r="I47" s="31" t="s">
+      <c r="I47" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="J47" s="31" t="s">
+      <c r="J47" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K47" s="31" t="s">
+      <c r="K47" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3719,32 +3727,32 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B48" s="30" t="s">
+      <c r="B48" s="25" t="s">
         <v>51</v>
       </c>
       <c r="C48" s="14">
         <v>2</v>
       </c>
-      <c r="D48" s="30" t="s">
+      <c r="D48" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="E48" s="30" t="s">
+      <c r="E48" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="F48" s="30" t="s">
+      <c r="F48" s="25" t="s">
         <v>170</v>
       </c>
-      <c r="G48" s="31" t="s">
+      <c r="G48" s="26" t="s">
         <v>260</v>
       </c>
       <c r="H48" s="15"/>
-      <c r="I48" s="31" t="s">
+      <c r="I48" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="J48" s="31" t="s">
+      <c r="J48" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K48" s="31" t="s">
+      <c r="K48" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3753,32 +3761,32 @@
         <f>ROW(A49) - ROW($A$10)</f>
         <v>39</v>
       </c>
-      <c r="B49" s="30" t="s">
+      <c r="B49" s="25" t="s">
         <v>52</v>
       </c>
       <c r="C49" s="14">
         <v>2</v>
       </c>
-      <c r="D49" s="30" t="s">
+      <c r="D49" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="E49" s="30" t="s">
+      <c r="E49" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="F49" s="30" t="s">
+      <c r="F49" s="25" t="s">
         <v>171</v>
       </c>
-      <c r="G49" s="31" t="s">
+      <c r="G49" s="26" t="s">
         <v>261</v>
       </c>
       <c r="H49" s="15"/>
-      <c r="I49" s="31" t="s">
+      <c r="I49" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J49" s="31" t="s">
+      <c r="J49" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K49" s="31" t="s">
+      <c r="K49" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3787,32 +3795,32 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B50" s="30" t="s">
+      <c r="B50" s="25" t="s">
         <v>53</v>
       </c>
       <c r="C50" s="14">
         <v>2</v>
       </c>
-      <c r="D50" s="30" t="s">
+      <c r="D50" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="E50" s="30" t="s">
+      <c r="E50" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="F50" s="30" t="s">
+      <c r="F50" s="25" t="s">
         <v>172</v>
       </c>
-      <c r="G50" s="31" t="s">
+      <c r="G50" s="26" t="s">
         <v>262</v>
       </c>
       <c r="H50" s="15"/>
-      <c r="I50" s="31" t="s">
+      <c r="I50" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="J50" s="31" t="s">
+      <c r="J50" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K50" s="31" t="s">
+      <c r="K50" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3821,32 +3829,32 @@
         <f>ROW(A51) - ROW($A$10)</f>
         <v>41</v>
       </c>
-      <c r="B51" s="30" t="s">
+      <c r="B51" s="25" t="s">
         <v>54</v>
       </c>
       <c r="C51" s="14">
         <v>2</v>
       </c>
-      <c r="D51" s="30" t="s">
+      <c r="D51" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="E51" s="30" t="s">
+      <c r="E51" s="25" t="s">
         <v>173</v>
       </c>
-      <c r="F51" s="30" t="s">
+      <c r="F51" s="25" t="s">
         <v>221</v>
       </c>
-      <c r="G51" s="31" t="s">
+      <c r="G51" s="26" t="s">
         <v>263</v>
       </c>
       <c r="H51" s="15"/>
-      <c r="I51" s="31" t="s">
+      <c r="I51" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="J51" s="31" t="s">
+      <c r="J51" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K51" s="31" t="s">
+      <c r="K51" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3855,32 +3863,32 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B52" s="30" t="s">
+      <c r="B52" s="25" t="s">
         <v>55</v>
       </c>
       <c r="C52" s="14">
         <v>2</v>
       </c>
-      <c r="D52" s="30" t="s">
+      <c r="D52" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="E52" s="30" t="s">
+      <c r="E52" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="F52" s="30" t="s">
+      <c r="F52" s="25" t="s">
         <v>174</v>
       </c>
-      <c r="G52" s="31" t="s">
+      <c r="G52" s="26" t="s">
         <v>264</v>
       </c>
       <c r="H52" s="15"/>
-      <c r="I52" s="31" t="s">
+      <c r="I52" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="J52" s="31" t="s">
+      <c r="J52" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K52" s="31" t="s">
+      <c r="K52" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3889,32 +3897,32 @@
         <f>ROW(A53) - ROW($A$10)</f>
         <v>43</v>
       </c>
-      <c r="B53" s="30" t="s">
+      <c r="B53" s="25" t="s">
         <v>56</v>
       </c>
       <c r="C53" s="14">
         <v>2</v>
       </c>
-      <c r="D53" s="30" t="s">
+      <c r="D53" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="E53" s="30" t="s">
+      <c r="E53" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="F53" s="30" t="s">
+      <c r="F53" s="25" t="s">
         <v>175</v>
       </c>
-      <c r="G53" s="31" t="s">
+      <c r="G53" s="26" t="s">
         <v>265</v>
       </c>
       <c r="H53" s="15"/>
-      <c r="I53" s="31" t="s">
+      <c r="I53" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J53" s="31" t="s">
+      <c r="J53" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K53" s="31" t="s">
+      <c r="K53" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3923,32 +3931,32 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="25" t="s">
         <v>57</v>
       </c>
       <c r="C54" s="14">
         <v>2</v>
       </c>
-      <c r="D54" s="30" t="s">
+      <c r="D54" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="E54" s="30" t="s">
+      <c r="E54" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="F54" s="30" t="s">
+      <c r="F54" s="25" t="s">
         <v>176</v>
       </c>
-      <c r="G54" s="31" t="s">
+      <c r="G54" s="26" t="s">
         <v>266</v>
       </c>
       <c r="H54" s="15"/>
-      <c r="I54" s="31" t="s">
+      <c r="I54" s="26" t="s">
         <v>326</v>
       </c>
-      <c r="J54" s="31" t="s">
+      <c r="J54" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K54" s="31" t="s">
+      <c r="K54" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3957,32 +3965,32 @@
         <f>ROW(A55) - ROW($A$10)</f>
         <v>45</v>
       </c>
-      <c r="B55" s="30" t="s">
+      <c r="B55" s="25" t="s">
         <v>58</v>
       </c>
       <c r="C55" s="14">
         <v>2</v>
       </c>
-      <c r="D55" s="30" t="s">
+      <c r="D55" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="E55" s="30" t="s">
+      <c r="E55" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="F55" s="30" t="s">
+      <c r="F55" s="25" t="s">
         <v>177</v>
       </c>
-      <c r="G55" s="31" t="s">
+      <c r="G55" s="26" t="s">
         <v>267</v>
       </c>
       <c r="H55" s="15"/>
-      <c r="I55" s="31" t="s">
+      <c r="I55" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J55" s="31" t="s">
+      <c r="J55" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K55" s="31" t="s">
+      <c r="K55" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -3991,32 +3999,32 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B56" s="30" t="s">
+      <c r="B56" s="25" t="s">
         <v>59</v>
       </c>
       <c r="C56" s="14">
         <v>2</v>
       </c>
-      <c r="D56" s="30" t="s">
+      <c r="D56" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="E56" s="30" t="s">
+      <c r="E56" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="F56" s="30" t="s">
+      <c r="F56" s="25" t="s">
         <v>178</v>
       </c>
-      <c r="G56" s="31" t="s">
+      <c r="G56" s="26" t="s">
         <v>268</v>
       </c>
       <c r="H56" s="15"/>
-      <c r="I56" s="31" t="s">
+      <c r="I56" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J56" s="31" t="s">
+      <c r="J56" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K56" s="31" t="s">
+      <c r="K56" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4025,32 +4033,32 @@
         <f>ROW(A57) - ROW($A$10)</f>
         <v>47</v>
       </c>
-      <c r="B57" s="30" t="s">
+      <c r="B57" s="25" t="s">
         <v>60</v>
       </c>
       <c r="C57" s="14">
         <v>2</v>
       </c>
-      <c r="D57" s="30" t="s">
+      <c r="D57" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="E57" s="30" t="s">
+      <c r="E57" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="F57" s="30" t="s">
+      <c r="F57" s="25" t="s">
         <v>179</v>
       </c>
-      <c r="G57" s="31" t="s">
+      <c r="G57" s="26" t="s">
         <v>269</v>
       </c>
       <c r="H57" s="15"/>
-      <c r="I57" s="31" t="s">
+      <c r="I57" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J57" s="31" t="s">
+      <c r="J57" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K57" s="31" t="s">
+      <c r="K57" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4059,32 +4067,32 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B58" s="25" t="s">
         <v>61</v>
       </c>
       <c r="C58" s="14">
         <v>2</v>
       </c>
-      <c r="D58" s="30" t="s">
+      <c r="D58" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="E58" s="30" t="s">
+      <c r="E58" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="F58" s="30" t="s">
+      <c r="F58" s="25" t="s">
         <v>180</v>
       </c>
-      <c r="G58" s="31" t="s">
+      <c r="G58" s="26" t="s">
         <v>270</v>
       </c>
       <c r="H58" s="15"/>
-      <c r="I58" s="31" t="s">
+      <c r="I58" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="J58" s="31" t="s">
+      <c r="J58" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K58" s="31" t="s">
+      <c r="K58" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4093,32 +4101,32 @@
         <f>ROW(A59) - ROW($A$10)</f>
         <v>49</v>
       </c>
-      <c r="B59" s="30" t="s">
+      <c r="B59" s="25" t="s">
         <v>62</v>
       </c>
       <c r="C59" s="14">
         <v>2</v>
       </c>
-      <c r="D59" s="30" t="s">
+      <c r="D59" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="E59" s="30" t="s">
+      <c r="E59" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="F59" s="30" t="s">
+      <c r="F59" s="25" t="s">
         <v>181</v>
       </c>
-      <c r="G59" s="31" t="s">
+      <c r="G59" s="26" t="s">
         <v>271</v>
       </c>
       <c r="H59" s="15"/>
-      <c r="I59" s="31" t="s">
+      <c r="I59" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J59" s="31" t="s">
+      <c r="J59" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K59" s="31" t="s">
+      <c r="K59" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4127,32 +4135,32 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B60" s="30" t="s">
+      <c r="B60" s="25" t="s">
         <v>63</v>
       </c>
       <c r="C60" s="14">
         <v>2</v>
       </c>
-      <c r="D60" s="30" t="s">
+      <c r="D60" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="E60" s="30" t="s">
+      <c r="E60" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="F60" s="30" t="s">
+      <c r="F60" s="25" t="s">
         <v>182</v>
       </c>
-      <c r="G60" s="31" t="s">
+      <c r="G60" s="26" t="s">
         <v>272</v>
       </c>
       <c r="H60" s="15"/>
-      <c r="I60" s="31" t="s">
+      <c r="I60" s="26" t="s">
         <v>317</v>
       </c>
-      <c r="J60" s="31" t="s">
+      <c r="J60" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K60" s="31" t="s">
+      <c r="K60" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4161,32 +4169,32 @@
         <f>ROW(A61) - ROW($A$10)</f>
         <v>51</v>
       </c>
-      <c r="B61" s="30" t="s">
+      <c r="B61" s="25" t="s">
         <v>64</v>
       </c>
       <c r="C61" s="14">
         <v>2</v>
       </c>
-      <c r="D61" s="30" t="s">
+      <c r="D61" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="E61" s="30" t="s">
+      <c r="E61" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="F61" s="30" t="s">
+      <c r="F61" s="25" t="s">
         <v>183</v>
       </c>
-      <c r="G61" s="31" t="s">
+      <c r="G61" s="26" t="s">
         <v>273</v>
       </c>
       <c r="H61" s="15"/>
-      <c r="I61" s="31" t="s">
+      <c r="I61" s="26" t="s">
         <v>183</v>
       </c>
-      <c r="J61" s="31" t="s">
+      <c r="J61" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="K61" s="31" t="s">
+      <c r="K61" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4195,32 +4203,32 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B62" s="30" t="s">
+      <c r="B62" s="25" t="s">
         <v>65</v>
       </c>
       <c r="C62" s="14">
         <v>2</v>
       </c>
-      <c r="D62" s="30" t="s">
+      <c r="D62" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E62" s="30" t="s">
+      <c r="E62" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="F62" s="30" t="s">
+      <c r="F62" s="25" t="s">
         <v>184</v>
       </c>
-      <c r="G62" s="31" t="s">
+      <c r="G62" s="26" t="s">
         <v>184</v>
       </c>
       <c r="H62" s="15"/>
-      <c r="I62" s="31" t="s">
+      <c r="I62" s="26" t="s">
         <v>327</v>
       </c>
-      <c r="J62" s="31" t="s">
+      <c r="J62" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K62" s="31" t="s">
+      <c r="K62" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4229,32 +4237,32 @@
         <f>ROW(A63) - ROW($A$10)</f>
         <v>53</v>
       </c>
-      <c r="B63" s="30" t="s">
+      <c r="B63" s="25" t="s">
         <v>66</v>
       </c>
       <c r="C63" s="14">
         <v>2</v>
       </c>
-      <c r="D63" s="30" t="s">
+      <c r="D63" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E63" s="30" t="s">
+      <c r="E63" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="F63" s="30" t="s">
+      <c r="F63" s="25" t="s">
         <v>185</v>
       </c>
-      <c r="G63" s="31" t="s">
+      <c r="G63" s="26" t="s">
         <v>185</v>
       </c>
       <c r="H63" s="15"/>
-      <c r="I63" s="31" t="s">
+      <c r="I63" s="26" t="s">
         <v>327</v>
       </c>
-      <c r="J63" s="31" t="s">
+      <c r="J63" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K63" s="31" t="s">
+      <c r="K63" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4263,32 +4271,32 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B64" s="30" t="s">
+      <c r="B64" s="25" t="s">
         <v>67</v>
       </c>
       <c r="C64" s="14">
         <v>1</v>
       </c>
-      <c r="D64" s="30" t="s">
+      <c r="D64" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E64" s="30" t="s">
+      <c r="E64" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="F64" s="30" t="s">
+      <c r="F64" s="25" t="s">
         <v>186</v>
       </c>
-      <c r="G64" s="31" t="s">
+      <c r="G64" s="26" t="s">
         <v>274</v>
       </c>
       <c r="H64" s="15"/>
-      <c r="I64" s="31" t="s">
+      <c r="I64" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="J64" s="31" t="s">
+      <c r="J64" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K64" s="31" t="s">
+      <c r="K64" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4297,32 +4305,32 @@
         <f>ROW(A65) - ROW($A$10)</f>
         <v>55</v>
       </c>
-      <c r="B65" s="30" t="s">
+      <c r="B65" s="25" t="s">
         <v>68</v>
       </c>
       <c r="C65" s="14">
         <v>1</v>
       </c>
-      <c r="D65" s="30" t="s">
+      <c r="D65" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="E65" s="30" t="s">
+      <c r="E65" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="F65" s="30" t="s">
+      <c r="F65" s="25" t="s">
         <v>187</v>
       </c>
-      <c r="G65" s="31" t="s">
+      <c r="G65" s="26" t="s">
         <v>275</v>
       </c>
       <c r="H65" s="15"/>
-      <c r="I65" s="31" t="s">
+      <c r="I65" s="26" t="s">
         <v>304</v>
       </c>
-      <c r="J65" s="31" t="s">
+      <c r="J65" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K65" s="31" t="s">
+      <c r="K65" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4331,32 +4339,32 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B66" s="30" t="s">
+      <c r="B66" s="25" t="s">
         <v>69</v>
       </c>
       <c r="C66" s="14">
         <v>1</v>
       </c>
-      <c r="D66" s="30" t="s">
+      <c r="D66" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="E66" s="30" t="s">
+      <c r="E66" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="F66" s="30" t="s">
+      <c r="F66" s="25" t="s">
         <v>188</v>
       </c>
-      <c r="G66" s="31" t="s">
+      <c r="G66" s="26" t="s">
         <v>276</v>
       </c>
       <c r="H66" s="15"/>
-      <c r="I66" s="31" t="s">
+      <c r="I66" s="26" t="s">
         <v>316</v>
       </c>
-      <c r="J66" s="31" t="s">
+      <c r="J66" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K66" s="31" t="s">
+      <c r="K66" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4365,32 +4373,32 @@
         <f>ROW(A67) - ROW($A$10)</f>
         <v>57</v>
       </c>
-      <c r="B67" s="30" t="s">
+      <c r="B67" s="25" t="s">
         <v>70</v>
       </c>
       <c r="C67" s="14">
         <v>1</v>
       </c>
-      <c r="D67" s="30" t="s">
+      <c r="D67" s="25" t="s">
         <v>121</v>
       </c>
-      <c r="E67" s="30" t="s">
+      <c r="E67" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="F67" s="30" t="s">
+      <c r="F67" s="25" t="s">
         <v>189</v>
       </c>
-      <c r="G67" s="31" t="s">
+      <c r="G67" s="26" t="s">
         <v>277</v>
       </c>
       <c r="H67" s="15"/>
-      <c r="I67" s="31" t="s">
+      <c r="I67" s="26" t="s">
         <v>305</v>
       </c>
-      <c r="J67" s="31" t="s">
+      <c r="J67" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K67" s="31" t="s">
+      <c r="K67" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4399,32 +4407,32 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B68" s="30" t="s">
+      <c r="B68" s="25" t="s">
         <v>71</v>
       </c>
       <c r="C68" s="14">
         <v>1</v>
       </c>
-      <c r="D68" s="30" t="s">
+      <c r="D68" s="25" t="s">
         <v>123</v>
       </c>
-      <c r="E68" s="30" t="s">
+      <c r="E68" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="F68" s="30" t="s">
+      <c r="F68" s="25" t="s">
         <v>190</v>
       </c>
-      <c r="G68" s="31" t="s">
+      <c r="G68" s="26" t="s">
         <v>278</v>
       </c>
       <c r="H68" s="15"/>
-      <c r="I68" s="31" t="s">
+      <c r="I68" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J68" s="31" t="s">
+      <c r="J68" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K68" s="31" t="s">
+      <c r="K68" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4433,32 +4441,32 @@
         <f>ROW(A69) - ROW($A$10)</f>
         <v>59</v>
       </c>
-      <c r="B69" s="30" t="s">
+      <c r="B69" s="25" t="s">
         <v>72</v>
       </c>
       <c r="C69" s="14">
         <v>1</v>
       </c>
-      <c r="D69" s="30" t="s">
+      <c r="D69" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="E69" s="30" t="s">
+      <c r="E69" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="F69" s="30" t="s">
+      <c r="F69" s="25" t="s">
         <v>191</v>
       </c>
-      <c r="G69" s="31" t="s">
+      <c r="G69" s="26" t="s">
         <v>279</v>
       </c>
       <c r="H69" s="15"/>
-      <c r="I69" s="31" t="s">
+      <c r="I69" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J69" s="31" t="s">
+      <c r="J69" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K69" s="31" t="s">
+      <c r="K69" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4467,32 +4475,32 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B70" s="30" t="s">
+      <c r="B70" s="25" t="s">
         <v>73</v>
       </c>
       <c r="C70" s="14">
         <v>1</v>
       </c>
-      <c r="D70" s="30" t="s">
+      <c r="D70" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E70" s="30" t="s">
+      <c r="E70" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="F70" s="30" t="s">
+      <c r="F70" s="25" t="s">
         <v>192</v>
       </c>
-      <c r="G70" s="31" t="s">
+      <c r="G70" s="26" t="s">
         <v>280</v>
       </c>
       <c r="H70" s="15"/>
-      <c r="I70" s="31" t="s">
+      <c r="I70" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J70" s="31" t="s">
+      <c r="J70" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K70" s="31" t="s">
+      <c r="K70" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4501,32 +4509,32 @@
         <f>ROW(A71) - ROW($A$10)</f>
         <v>61</v>
       </c>
-      <c r="B71" s="30" t="s">
+      <c r="B71" s="25" t="s">
         <v>74</v>
       </c>
       <c r="C71" s="14">
         <v>1</v>
       </c>
-      <c r="D71" s="30" t="s">
+      <c r="D71" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="E71" s="30" t="s">
+      <c r="E71" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="F71" s="30" t="s">
+      <c r="F71" s="25" t="s">
         <v>193</v>
       </c>
-      <c r="G71" s="31" t="s">
+      <c r="G71" s="26" t="s">
         <v>281</v>
       </c>
       <c r="H71" s="15"/>
-      <c r="I71" s="31" t="s">
+      <c r="I71" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J71" s="31" t="s">
+      <c r="J71" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K71" s="31" t="s">
+      <c r="K71" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4535,32 +4543,32 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B72" s="30" t="s">
+      <c r="B72" s="25" t="s">
         <v>75</v>
       </c>
       <c r="C72" s="14">
         <v>1</v>
       </c>
-      <c r="D72" s="30" t="s">
+      <c r="D72" s="25" t="s">
         <v>127</v>
       </c>
-      <c r="E72" s="30" t="s">
+      <c r="E72" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="F72" s="30" t="s">
+      <c r="F72" s="25" t="s">
         <v>194</v>
       </c>
-      <c r="G72" s="31" t="s">
+      <c r="G72" s="26" t="s">
         <v>282</v>
       </c>
       <c r="H72" s="15"/>
-      <c r="I72" s="31" t="s">
+      <c r="I72" s="26" t="s">
         <v>328</v>
       </c>
-      <c r="J72" s="31" t="s">
+      <c r="J72" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K72" s="31" t="s">
+      <c r="K72" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4569,32 +4577,32 @@
         <f>ROW(A73) - ROW($A$10)</f>
         <v>63</v>
       </c>
-      <c r="B73" s="30" t="s">
+      <c r="B73" s="25" t="s">
         <v>76</v>
       </c>
       <c r="C73" s="14">
         <v>1</v>
       </c>
-      <c r="D73" s="30" t="s">
+      <c r="D73" s="25" t="s">
         <v>104</v>
       </c>
-      <c r="E73" s="30" t="s">
+      <c r="E73" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="F73" s="30" t="s">
+      <c r="F73" s="25" t="s">
         <v>195</v>
       </c>
-      <c r="G73" s="31" t="s">
+      <c r="G73" s="26" t="s">
         <v>283</v>
       </c>
       <c r="H73" s="15"/>
-      <c r="I73" s="31" t="s">
+      <c r="I73" s="26" t="s">
         <v>325</v>
       </c>
-      <c r="J73" s="31" t="s">
+      <c r="J73" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K73" s="31" t="s">
+      <c r="K73" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4603,32 +4611,32 @@
         <f t="shared" si="0"/>
         <v>64</v>
       </c>
-      <c r="B74" s="30" t="s">
+      <c r="B74" s="25" t="s">
         <v>77</v>
       </c>
       <c r="C74" s="14">
         <v>1</v>
       </c>
-      <c r="D74" s="30" t="s">
+      <c r="D74" s="25" t="s">
         <v>103</v>
       </c>
-      <c r="E74" s="30" t="s">
+      <c r="E74" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="F74" s="30" t="s">
+      <c r="F74" s="25" t="s">
         <v>196</v>
       </c>
-      <c r="G74" s="31" t="s">
+      <c r="G74" s="26" t="s">
         <v>284</v>
       </c>
       <c r="H74" s="15"/>
-      <c r="I74" s="31" t="s">
+      <c r="I74" s="26" t="s">
         <v>329</v>
       </c>
-      <c r="J74" s="31" t="s">
+      <c r="J74" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K74" s="31" t="s">
+      <c r="K74" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4637,32 +4645,32 @@
         <f>ROW(A75) - ROW($A$10)</f>
         <v>65</v>
       </c>
-      <c r="B75" s="30" t="s">
+      <c r="B75" s="25" t="s">
         <v>78</v>
       </c>
       <c r="C75" s="14">
         <v>1</v>
       </c>
-      <c r="D75" s="30" t="s">
+      <c r="D75" s="25" t="s">
         <v>128</v>
       </c>
-      <c r="E75" s="30" t="s">
+      <c r="E75" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="F75" s="30" t="s">
+      <c r="F75" s="25" t="s">
         <v>197</v>
       </c>
-      <c r="G75" s="31" t="s">
+      <c r="G75" s="26" t="s">
         <v>285</v>
       </c>
       <c r="H75" s="15"/>
-      <c r="I75" s="31" t="s">
+      <c r="I75" s="26" t="s">
         <v>330</v>
       </c>
-      <c r="J75" s="31" t="s">
+      <c r="J75" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K75" s="31" t="s">
+      <c r="K75" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4671,32 +4679,32 @@
         <f t="shared" si="0"/>
         <v>66</v>
       </c>
-      <c r="B76" s="30" t="s">
+      <c r="B76" s="25" t="s">
         <v>79</v>
       </c>
       <c r="C76" s="14">
         <v>1</v>
       </c>
-      <c r="D76" s="30" t="s">
+      <c r="D76" s="25" t="s">
         <v>129</v>
       </c>
-      <c r="E76" s="30" t="s">
+      <c r="E76" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="F76" s="30" t="s">
+      <c r="F76" s="25" t="s">
         <v>198</v>
       </c>
-      <c r="G76" s="31" t="s">
+      <c r="G76" s="26" t="s">
         <v>286</v>
       </c>
       <c r="H76" s="15"/>
-      <c r="I76" s="31" t="s">
+      <c r="I76" s="26" t="s">
         <v>331</v>
       </c>
-      <c r="J76" s="31" t="s">
+      <c r="J76" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K76" s="31" t="s">
+      <c r="K76" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4705,32 +4713,32 @@
         <f>ROW(A77) - ROW($A$10)</f>
         <v>67</v>
       </c>
-      <c r="B77" s="30" t="s">
+      <c r="B77" s="25" t="s">
         <v>80</v>
       </c>
       <c r="C77" s="14">
         <v>1</v>
       </c>
-      <c r="D77" s="30" t="s">
+      <c r="D77" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E77" s="30" t="s">
+      <c r="E77" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="F77" s="30" t="s">
+      <c r="F77" s="25" t="s">
         <v>199</v>
       </c>
-      <c r="G77" s="31" t="s">
+      <c r="G77" s="26" t="s">
         <v>287</v>
       </c>
       <c r="H77" s="15"/>
-      <c r="I77" s="31" t="s">
+      <c r="I77" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J77" s="31" t="s">
+      <c r="J77" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K77" s="31" t="s">
+      <c r="K77" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4739,32 +4747,32 @@
         <f t="shared" si="0"/>
         <v>68</v>
       </c>
-      <c r="B78" s="30" t="s">
+      <c r="B78" s="25" t="s">
         <v>81</v>
       </c>
       <c r="C78" s="14">
         <v>1</v>
       </c>
-      <c r="D78" s="30" t="s">
+      <c r="D78" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="E78" s="30" t="s">
+      <c r="E78" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="F78" s="30" t="s">
+      <c r="F78" s="25" t="s">
         <v>200</v>
       </c>
-      <c r="G78" s="31" t="s">
+      <c r="G78" s="26" t="s">
         <v>288</v>
       </c>
       <c r="H78" s="15"/>
-      <c r="I78" s="31" t="s">
+      <c r="I78" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J78" s="31" t="s">
+      <c r="J78" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K78" s="31" t="s">
+      <c r="K78" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4773,32 +4781,32 @@
         <f>ROW(A79) - ROW($A$10)</f>
         <v>69</v>
       </c>
-      <c r="B79" s="30" t="s">
+      <c r="B79" s="25" t="s">
         <v>82</v>
       </c>
       <c r="C79" s="14">
         <v>1</v>
       </c>
-      <c r="D79" s="30" t="s">
+      <c r="D79" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="E79" s="30" t="s">
+      <c r="E79" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="F79" s="30" t="s">
+      <c r="F79" s="25" t="s">
         <v>201</v>
       </c>
-      <c r="G79" s="31" t="s">
+      <c r="G79" s="26" t="s">
         <v>289</v>
       </c>
       <c r="H79" s="15"/>
-      <c r="I79" s="31" t="s">
+      <c r="I79" s="26" t="s">
         <v>308</v>
       </c>
-      <c r="J79" s="31" t="s">
+      <c r="J79" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K79" s="31" t="s">
+      <c r="K79" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4807,32 +4815,32 @@
         <f t="shared" si="0"/>
         <v>70</v>
       </c>
-      <c r="B80" s="30" t="s">
+      <c r="B80" s="25" t="s">
         <v>83</v>
       </c>
       <c r="C80" s="14">
         <v>1</v>
       </c>
-      <c r="D80" s="30" t="s">
+      <c r="D80" s="25" t="s">
         <v>120</v>
       </c>
-      <c r="E80" s="30" t="s">
+      <c r="E80" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="F80" s="30" t="s">
+      <c r="F80" s="25" t="s">
         <v>202</v>
       </c>
-      <c r="G80" s="31" t="s">
+      <c r="G80" s="26" t="s">
         <v>290</v>
       </c>
       <c r="H80" s="15"/>
-      <c r="I80" s="31" t="s">
+      <c r="I80" s="26" t="s">
         <v>307</v>
       </c>
-      <c r="J80" s="31" t="s">
+      <c r="J80" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K80" s="31" t="s">
+      <c r="K80" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4841,32 +4849,32 @@
         <f>ROW(A81) - ROW($A$10)</f>
         <v>71</v>
       </c>
-      <c r="B81" s="30" t="s">
+      <c r="B81" s="25" t="s">
         <v>84</v>
       </c>
       <c r="C81" s="14">
         <v>1</v>
       </c>
-      <c r="D81" s="30" t="s">
+      <c r="D81" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E81" s="30" t="s">
+      <c r="E81" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="F81" s="30" t="s">
+      <c r="F81" s="25" t="s">
         <v>222</v>
       </c>
-      <c r="G81" s="31" t="s">
+      <c r="G81" s="26" t="s">
         <v>291</v>
       </c>
       <c r="H81" s="15"/>
-      <c r="I81" s="31" t="s">
+      <c r="I81" s="26" t="s">
         <v>332</v>
       </c>
-      <c r="J81" s="31" t="s">
+      <c r="J81" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K81" s="31" t="s">
+      <c r="K81" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4875,32 +4883,32 @@
         <f t="shared" si="0"/>
         <v>72</v>
       </c>
-      <c r="B82" s="30" t="s">
+      <c r="B82" s="25" t="s">
         <v>85</v>
       </c>
       <c r="C82" s="14">
         <v>1</v>
       </c>
-      <c r="D82" s="30" t="s">
+      <c r="D82" s="25" t="s">
         <v>111</v>
       </c>
-      <c r="E82" s="30" t="s">
+      <c r="E82" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="F82" s="30" t="s">
+      <c r="F82" s="25" t="s">
         <v>204</v>
       </c>
-      <c r="G82" s="31" t="s">
+      <c r="G82" s="26" t="s">
         <v>292</v>
       </c>
       <c r="H82" s="15"/>
-      <c r="I82" s="31" t="s">
+      <c r="I82" s="26" t="s">
         <v>333</v>
       </c>
-      <c r="J82" s="31" t="s">
+      <c r="J82" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K82" s="31" t="s">
+      <c r="K82" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4909,32 +4917,32 @@
         <f>ROW(A83) - ROW($A$10)</f>
         <v>73</v>
       </c>
-      <c r="B83" s="30" t="s">
+      <c r="B83" s="25" t="s">
         <v>86</v>
       </c>
       <c r="C83" s="14">
         <v>1</v>
       </c>
-      <c r="D83" s="30" t="s">
+      <c r="D83" s="25" t="s">
         <v>130</v>
       </c>
-      <c r="E83" s="30" t="s">
+      <c r="E83" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="F83" s="30" t="s">
+      <c r="F83" s="25" t="s">
         <v>205</v>
       </c>
-      <c r="G83" s="31" t="s">
+      <c r="G83" s="26" t="s">
         <v>293</v>
       </c>
       <c r="H83" s="15"/>
-      <c r="I83" s="31" t="s">
+      <c r="I83" s="26" t="s">
         <v>334</v>
       </c>
-      <c r="J83" s="31" t="s">
+      <c r="J83" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K83" s="31" t="s">
+      <c r="K83" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4943,32 +4951,32 @@
         <f t="shared" si="0"/>
         <v>74</v>
       </c>
-      <c r="B84" s="30" t="s">
+      <c r="B84" s="25" t="s">
         <v>87</v>
       </c>
       <c r="C84" s="14">
         <v>1</v>
       </c>
-      <c r="D84" s="30" t="s">
+      <c r="D84" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="E84" s="30" t="s">
+      <c r="E84" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="F84" s="30" t="s">
+      <c r="F84" s="25" t="s">
         <v>206</v>
       </c>
-      <c r="G84" s="31" t="s">
+      <c r="G84" s="26" t="s">
         <v>294</v>
       </c>
       <c r="H84" s="15"/>
-      <c r="I84" s="31" t="s">
+      <c r="I84" s="26" t="s">
         <v>335</v>
       </c>
-      <c r="J84" s="31" t="s">
+      <c r="J84" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="K84" s="31" t="s">
+      <c r="K84" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -4977,32 +4985,32 @@
         <f>ROW(A85) - ROW($A$10)</f>
         <v>75</v>
       </c>
-      <c r="B85" s="30" t="s">
+      <c r="B85" s="25" t="s">
         <v>88</v>
       </c>
       <c r="C85" s="14">
         <v>1</v>
       </c>
-      <c r="D85" s="30" t="s">
+      <c r="D85" s="25" t="s">
         <v>122</v>
       </c>
-      <c r="E85" s="30" t="s">
+      <c r="E85" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="F85" s="30" t="s">
+      <c r="F85" s="25" t="s">
         <v>207</v>
       </c>
-      <c r="G85" s="31" t="s">
+      <c r="G85" s="26" t="s">
         <v>295</v>
       </c>
       <c r="H85" s="15"/>
-      <c r="I85" s="31" t="s">
+      <c r="I85" s="26" t="s">
         <v>207</v>
       </c>
-      <c r="J85" s="31" t="s">
+      <c r="J85" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K85" s="31" t="s">
+      <c r="K85" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5011,32 +5019,32 @@
         <f t="shared" si="0"/>
         <v>76</v>
       </c>
-      <c r="B86" s="30" t="s">
+      <c r="B86" s="25" t="s">
         <v>89</v>
       </c>
       <c r="C86" s="14">
         <v>1</v>
       </c>
-      <c r="D86" s="30" t="s">
+      <c r="D86" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="E86" s="30" t="s">
+      <c r="E86" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="F86" s="30" t="s">
+      <c r="F86" s="25" t="s">
         <v>208</v>
       </c>
-      <c r="G86" s="31" t="s">
+      <c r="G86" s="26" t="s">
         <v>296</v>
       </c>
       <c r="H86" s="15"/>
-      <c r="I86" s="31" t="s">
+      <c r="I86" s="26" t="s">
         <v>336</v>
       </c>
-      <c r="J86" s="31" t="s">
+      <c r="J86" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K86" s="31" t="s">
+      <c r="K86" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5045,32 +5053,32 @@
         <f>ROW(A87) - ROW($A$10)</f>
         <v>77</v>
       </c>
-      <c r="B87" s="30" t="s">
+      <c r="B87" s="25" t="s">
         <v>90</v>
       </c>
       <c r="C87" s="14">
         <v>1</v>
       </c>
-      <c r="D87" s="30" t="s">
+      <c r="D87" s="25" t="s">
         <v>124</v>
       </c>
-      <c r="E87" s="30" t="s">
+      <c r="E87" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="F87" s="30" t="s">
+      <c r="F87" s="25" t="s">
         <v>209</v>
       </c>
-      <c r="G87" s="31" t="s">
+      <c r="G87" s="26" t="s">
         <v>297</v>
       </c>
       <c r="H87" s="15"/>
-      <c r="I87" s="31" t="s">
+      <c r="I87" s="26" t="s">
         <v>337</v>
       </c>
-      <c r="J87" s="31" t="s">
+      <c r="J87" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K87" s="31" t="s">
+      <c r="K87" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5079,32 +5087,32 @@
         <f t="shared" si="0"/>
         <v>78</v>
       </c>
-      <c r="B88" s="30" t="s">
+      <c r="B88" s="25" t="s">
         <v>91</v>
       </c>
       <c r="C88" s="14">
         <v>1</v>
       </c>
-      <c r="D88" s="30" t="s">
+      <c r="D88" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E88" s="30" t="s">
+      <c r="E88" s="25" t="s">
         <v>210</v>
       </c>
-      <c r="F88" s="30" t="s">
+      <c r="F88" s="25" t="s">
         <v>223</v>
       </c>
-      <c r="G88" s="31" t="s">
+      <c r="G88" s="26" t="s">
         <v>298</v>
       </c>
       <c r="H88" s="15"/>
-      <c r="I88" s="31" t="s">
+      <c r="I88" s="26" t="s">
         <v>338</v>
       </c>
-      <c r="J88" s="31" t="s">
+      <c r="J88" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K88" s="31" t="s">
+      <c r="K88" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5113,32 +5121,32 @@
         <f>ROW(A89) - ROW($A$10)</f>
         <v>79</v>
       </c>
-      <c r="B89" s="30" t="s">
+      <c r="B89" s="25" t="s">
         <v>92</v>
       </c>
       <c r="C89" s="14">
-        <v>1</v>
-      </c>
-      <c r="D89" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D89" s="25" t="s">
         <v>125</v>
       </c>
-      <c r="E89" s="30" t="s">
+      <c r="E89" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="F89" s="30" t="s">
+      <c r="F89" s="25" t="s">
         <v>211</v>
       </c>
-      <c r="G89" s="31" t="s">
+      <c r="G89" s="26" t="s">
         <v>92</v>
       </c>
       <c r="H89" s="15"/>
-      <c r="I89" s="31" t="s">
+      <c r="I89" s="26" t="s">
         <v>92</v>
       </c>
-      <c r="J89" s="31" t="s">
+      <c r="J89" s="26" t="s">
         <v>342</v>
       </c>
-      <c r="K89" s="31" t="s">
+      <c r="K89" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5147,32 +5155,32 @@
         <f t="shared" si="0"/>
         <v>80</v>
       </c>
-      <c r="B90" s="30" t="s">
+      <c r="B90" s="25" t="s">
         <v>93</v>
       </c>
       <c r="C90" s="14">
         <v>1</v>
       </c>
-      <c r="D90" s="30" t="s">
+      <c r="D90" s="25" t="s">
         <v>132</v>
       </c>
-      <c r="E90" s="30" t="s">
+      <c r="E90" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="F90" s="30" t="s">
+      <c r="F90" s="25" t="s">
         <v>212</v>
       </c>
-      <c r="G90" s="31" t="s">
+      <c r="G90" s="26" t="s">
         <v>299</v>
       </c>
       <c r="H90" s="15"/>
-      <c r="I90" s="31" t="s">
+      <c r="I90" s="26" t="s">
         <v>311</v>
       </c>
-      <c r="J90" s="31" t="s">
+      <c r="J90" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K90" s="31" t="s">
+      <c r="K90" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5181,32 +5189,32 @@
         <f>ROW(A91) - ROW($A$10)</f>
         <v>81</v>
       </c>
-      <c r="B91" s="30" t="s">
+      <c r="B91" s="25" t="s">
         <v>94</v>
       </c>
       <c r="C91" s="14">
         <v>1</v>
       </c>
-      <c r="D91" s="30" t="s">
+      <c r="D91" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E91" s="30" t="s">
+      <c r="E91" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="F91" s="30" t="s">
+      <c r="F91" s="25" t="s">
         <v>213</v>
       </c>
-      <c r="G91" s="31" t="s">
+      <c r="G91" s="26" t="s">
         <v>300</v>
       </c>
       <c r="H91" s="15"/>
-      <c r="I91" s="31" t="s">
+      <c r="I91" s="26" t="s">
         <v>339</v>
       </c>
-      <c r="J91" s="31" t="s">
+      <c r="J91" s="26" t="s">
         <v>114</v>
       </c>
-      <c r="K91" s="31" t="s">
+      <c r="K91" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5215,32 +5223,32 @@
         <f t="shared" si="0"/>
         <v>82</v>
       </c>
-      <c r="B92" s="30" t="s">
+      <c r="B92" s="25" t="s">
         <v>95</v>
       </c>
       <c r="C92" s="14">
         <v>1</v>
       </c>
-      <c r="D92" s="30" t="s">
+      <c r="D92" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E92" s="30" t="s">
+      <c r="E92" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="F92" s="30" t="s">
+      <c r="F92" s="25" t="s">
         <v>214</v>
       </c>
-      <c r="G92" s="31" t="s">
+      <c r="G92" s="26" t="s">
         <v>301</v>
       </c>
       <c r="H92" s="15"/>
-      <c r="I92" s="31" t="s">
+      <c r="I92" s="26" t="s">
         <v>337</v>
       </c>
-      <c r="J92" s="31" t="s">
+      <c r="J92" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K92" s="31" t="s">
+      <c r="K92" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5249,32 +5257,32 @@
         <f>ROW(A93) - ROW($A$10)</f>
         <v>83</v>
       </c>
-      <c r="B93" s="30" t="s">
+      <c r="B93" s="25" t="s">
         <v>96</v>
       </c>
       <c r="C93" s="14">
         <v>1</v>
       </c>
-      <c r="D93" s="30" t="s">
+      <c r="D93" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E93" s="30" t="s">
+      <c r="E93" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="F93" s="30" t="s">
+      <c r="F93" s="25" t="s">
         <v>215</v>
       </c>
-      <c r="G93" s="31" t="s">
+      <c r="G93" s="26" t="s">
         <v>215</v>
       </c>
       <c r="H93" s="15"/>
-      <c r="I93" s="31" t="s">
+      <c r="I93" s="26" t="s">
         <v>327</v>
       </c>
-      <c r="J93" s="31" t="s">
+      <c r="J93" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K93" s="31" t="s">
+      <c r="K93" s="26" t="s">
         <v>343</v>
       </c>
     </row>
@@ -5283,32 +5291,32 @@
         <f t="shared" si="0"/>
         <v>84</v>
       </c>
-      <c r="B94" s="30" t="s">
+      <c r="B94" s="25" t="s">
         <v>97</v>
       </c>
       <c r="C94" s="14">
         <v>1</v>
       </c>
-      <c r="D94" s="30" t="s">
+      <c r="D94" s="25" t="s">
         <v>113</v>
       </c>
-      <c r="E94" s="30" t="s">
+      <c r="E94" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="F94" s="30" t="s">
+      <c r="F94" s="25" t="s">
         <v>216</v>
       </c>
-      <c r="G94" s="31" t="s">
+      <c r="G94" s="26" t="s">
         <v>216</v>
       </c>
       <c r="H94" s="15"/>
-      <c r="I94" s="31" t="s">
+      <c r="I94" s="26" t="s">
         <v>327</v>
       </c>
-      <c r="J94" s="31" t="s">
+      <c r="J94" s="26" t="s">
         <v>341</v>
       </c>
-      <c r="K94" s="31" t="s">
+      <c r="K94" s="26" t="s">
         <v>343</v>
       </c>
     </row>

</xml_diff>

<commit_message>
hardware: Updating all files for the new release
</commit_message>
<xml_diff>
--- a/hardware/fabrication/board_bom.xlsx
+++ b/hardware/fabrication/board_bom.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="403">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="405">
   <si>
     <t>Comment</t>
   </si>
@@ -405,580 +405,586 @@
     <t>GRM31CR71E106KA12L</t>
   </si>
   <si>
+    <t>47k, DNP</t>
+  </si>
+  <si>
+    <t>RES 47k OHM 1/10W 1% 0805</t>
+  </si>
+  <si>
+    <t>V1, V2, V3, V4</t>
+  </si>
+  <si>
+    <t>RC0805FR-0747KL</t>
+  </si>
+  <si>
+    <t>150R</t>
+  </si>
+  <si>
+    <t>RES 150R OHM 1/10W 1% 0603</t>
+  </si>
+  <si>
+    <t>R33, R42, R44, R92</t>
+  </si>
+  <si>
+    <t>CRCW0603150RFKEA</t>
+  </si>
+  <si>
+    <t>220uF/6.3V</t>
+  </si>
+  <si>
+    <t>CAP Tantalum 220uF 6.3V 20% 1210</t>
+  </si>
+  <si>
+    <t>C24, C31, C49, C56</t>
+  </si>
+  <si>
+    <t>6TPE220MAZB</t>
+  </si>
+  <si>
+    <t>cc1210</t>
+  </si>
+  <si>
+    <t>Panasonic</t>
+  </si>
+  <si>
+    <t>MOSFET-P-SI4403CDY-T1-GE3</t>
+  </si>
+  <si>
+    <t>MOSFET 1.8V P-Channel 20 V, 0.0155 Ω typ., 13.4 A</t>
+  </si>
+  <si>
+    <t>Q3, Q4, Q5, Q6</t>
+  </si>
+  <si>
+    <t>SI4403CDY-T1-GE3</t>
+  </si>
+  <si>
+    <t>5K9</t>
+  </si>
+  <si>
+    <t>RES 5K9 OHM 1/8W 1% 0805</t>
+  </si>
+  <si>
+    <t>R19, R24, R54</t>
+  </si>
+  <si>
+    <t>71-CRCW0805-5.9K-E3</t>
+  </si>
+  <si>
+    <t>CRCW08055K90FKEA</t>
+  </si>
+  <si>
+    <t>93K1</t>
+  </si>
+  <si>
+    <t>RES 93.1K OHM 1/10W 1% 0603</t>
+  </si>
+  <si>
+    <t>R69, R74, R81</t>
+  </si>
+  <si>
+    <t>CRCW060393K1FKEA</t>
+  </si>
+  <si>
+    <t>100uH/2.2/150.2mOHM</t>
+  </si>
+  <si>
+    <t>MSS1278T-104MLD - 100uH / 2.2A / 150.2mOHM</t>
+  </si>
+  <si>
+    <t>L7, L8, L9</t>
+  </si>
+  <si>
+    <t>IND_HC9</t>
+  </si>
+  <si>
+    <t>0532610671</t>
+  </si>
+  <si>
+    <t>PicoBlade 6 Position Right Angle Connector Header Surface Mount  0.049" (1.25mm)</t>
+  </si>
+  <si>
+    <t>SBW, SW1, SW2</t>
+  </si>
+  <si>
+    <t>53398-0671</t>
+  </si>
+  <si>
+    <t>PICOBLADE 6PIN Right Angle</t>
+  </si>
+  <si>
+    <t>0532610871</t>
+  </si>
+  <si>
+    <t>PicoBlade 8 Position Right Angle Connector Header Surface Mount 0.049" (1.25mm)</t>
+  </si>
+  <si>
+    <t>P8, RTD1, RTD2</t>
+  </si>
+  <si>
+    <t>53261-0871</t>
+  </si>
+  <si>
+    <t>PICOBLADE 8PIN RIGHT ANGLE</t>
+  </si>
+  <si>
+    <t>0.47uF/50V</t>
+  </si>
+  <si>
+    <t>CAP CER 0.47UF 50V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>C39, C65</t>
+  </si>
+  <si>
+    <t>C1608X7R1H474K080AE</t>
+  </si>
+  <si>
+    <t>TDK</t>
+  </si>
+  <si>
+    <t>RES SMD 1K OHM 1% 1/8W 0805</t>
+  </si>
+  <si>
+    <t>R25, R26</t>
+  </si>
+  <si>
+    <t>ERJ-6ENF1001V</t>
+  </si>
+  <si>
+    <t>2.2uH/9A 15mOHM</t>
+  </si>
+  <si>
+    <t>INDUCTOR 2.2UH 9A SMD</t>
+  </si>
+  <si>
+    <t>L1, L2</t>
+  </si>
+  <si>
+    <t>SRP6540-2R2M</t>
+  </si>
+  <si>
+    <t>Ind_SRP6540</t>
+  </si>
+  <si>
+    <t>Bourns</t>
+  </si>
+  <si>
+    <t>3SMAJ5919B-TP, DNP</t>
+  </si>
+  <si>
+    <t>DIODE ZENER 5.6V 3W DO214AC</t>
+  </si>
+  <si>
+    <t>D5, D6</t>
+  </si>
+  <si>
+    <t>3SMAJ5919B-TP</t>
+  </si>
+  <si>
+    <t>MCC</t>
+  </si>
+  <si>
+    <t>5.6nF/100V</t>
+  </si>
+  <si>
+    <t>CAP CER 5.6nF 100V 0603</t>
+  </si>
+  <si>
+    <t>C10, C20</t>
+  </si>
+  <si>
+    <t>C1608C0G2A562J080AE</t>
+  </si>
+  <si>
+    <t>10pF/100V</t>
+  </si>
+  <si>
+    <t>CAP CER 10pF 100V 0805</t>
+  </si>
+  <si>
+    <t>C68, C70</t>
+  </si>
+  <si>
+    <t>08051A100FAT2A</t>
+  </si>
+  <si>
+    <t>11.5k</t>
+  </si>
+  <si>
+    <t>RES 11.5k OHM 1/8W 1% 0805</t>
+  </si>
+  <si>
+    <t>R6, R13</t>
+  </si>
+  <si>
+    <t>AC0805FR-0711K5L</t>
+  </si>
+  <si>
+    <t>12pF/50V</t>
+  </si>
+  <si>
+    <t>CAP CER 12pF 50V 0603</t>
+  </si>
+  <si>
+    <t>C67, C69</t>
+  </si>
+  <si>
+    <t>GQM1885C1H120GB01D</t>
+  </si>
+  <si>
+    <t>13pF/50V</t>
+  </si>
+  <si>
+    <t>CAP CER 13PF 50V 0603 NP0</t>
+  </si>
+  <si>
+    <t>C9, C19</t>
+  </si>
+  <si>
+    <t>C0603C130J5GAC7867</t>
+  </si>
+  <si>
+    <t>KEMET</t>
+  </si>
+  <si>
+    <t>C0603C130J5GACTU</t>
+  </si>
+  <si>
+    <t>16uH/5A/34.5mOHM</t>
+  </si>
+  <si>
+    <t>INDUCTOR 16UH 5A SMD</t>
+  </si>
+  <si>
+    <t>L4, L5</t>
+  </si>
+  <si>
+    <t>7443251600</t>
+  </si>
+  <si>
+    <t>IND_744325xxx</t>
+  </si>
+  <si>
+    <t>19.6k</t>
+  </si>
+  <si>
+    <t>RES 19.6k OHM 1/10W 1% 0603</t>
+  </si>
+  <si>
+    <t>R5, R12</t>
+  </si>
+  <si>
+    <t>ERJ-3EKF1962V</t>
+  </si>
+  <si>
+    <t>30R@100Mhz, 10A</t>
+  </si>
+  <si>
+    <t>Ferrite Bead 30 OHM 10A 100MHz</t>
+  </si>
+  <si>
+    <t>FB3, FB4</t>
+  </si>
+  <si>
+    <t>BLE32PN300SN1L</t>
+  </si>
+  <si>
+    <t>IND1210</t>
+  </si>
+  <si>
+    <t>100K 1/10W</t>
+  </si>
+  <si>
+    <t>RES 100K OHM 1/10W 0.1% 0805</t>
+  </si>
+  <si>
+    <t>R35, R85</t>
+  </si>
+  <si>
+    <t>CPF-A-0805B100KE</t>
+  </si>
+  <si>
+    <t>TE Connectivity</t>
+  </si>
+  <si>
+    <t>140k</t>
+  </si>
+  <si>
+    <t>RES 140k OHM 1/5W 1% 0603</t>
+  </si>
+  <si>
+    <t>R7, R14</t>
+  </si>
+  <si>
+    <t>ERJ-P03F1403V</t>
+  </si>
+  <si>
+    <t>300K</t>
+  </si>
+  <si>
+    <t>RES 300K OHM 1/10W 0.1% 0603</t>
+  </si>
+  <si>
+    <t>R45, R70</t>
+  </si>
+  <si>
+    <t>RG1608P-304-B-T5</t>
+  </si>
+  <si>
+    <t>Susumu</t>
+  </si>
+  <si>
+    <t>1000pF/50V</t>
+  </si>
+  <si>
+    <t>CAP CER 1000pF 50V 10% X7R 0603</t>
+  </si>
+  <si>
+    <t>C37, C38</t>
+  </si>
+  <si>
+    <t>CC0603KRX7R9BB102</t>
+  </si>
+  <si>
+    <t>FSV530AF</t>
+  </si>
+  <si>
+    <t>DIODE SCHOTTKY 30V 5A DO-214AA</t>
+  </si>
+  <si>
+    <t>D1, D2</t>
+  </si>
+  <si>
+    <t>ON Semiconductor / Fairchild</t>
+  </si>
+  <si>
+    <t>Header 5X2IPS1-105-01-S-D</t>
+  </si>
+  <si>
+    <t>10 Position Receptacle Connector 0.100" (2.54mm)</t>
+  </si>
+  <si>
+    <t>P1, P5</t>
+  </si>
+  <si>
+    <t>IPS1-105-01-S-D</t>
+  </si>
+  <si>
+    <t>Samtec</t>
+  </si>
+  <si>
+    <t>Through Hole</t>
+  </si>
+  <si>
+    <t>TPS5420QDRQ1</t>
+  </si>
+  <si>
+    <t>U4, U9</t>
+  </si>
+  <si>
+    <t>SO8 Power PAD</t>
+  </si>
+  <si>
+    <t>TPS54540QDDARQ1</t>
+  </si>
+  <si>
+    <t>U2, U14</t>
+  </si>
+  <si>
+    <t>0.01R/0.5W</t>
+  </si>
+  <si>
+    <t>Current Sense Resistors - SMD 0.01ohm .5% 4 Terminal</t>
+  </si>
+  <si>
+    <t>RSense1</t>
+  </si>
+  <si>
+    <t>LVK12R010DER</t>
+  </si>
+  <si>
+    <t>0.01uF/25V</t>
+  </si>
+  <si>
+    <t>CAP CER 0.01UF 25V 5% X7R 0603</t>
+  </si>
+  <si>
+    <t>C66</t>
+  </si>
+  <si>
+    <t>06033C103JAT4A</t>
+  </si>
+  <si>
+    <t>0.075R/0.5W</t>
+  </si>
+  <si>
+    <t>Current Sense Resistors - SMD 1/2W 0.075 OHMS 1% 4 Terminal</t>
+  </si>
+  <si>
+    <t>Rsense3</t>
+  </si>
+  <si>
+    <t>LVK12R075FER</t>
+  </si>
+  <si>
+    <t>1nF/16V</t>
+  </si>
+  <si>
+    <t>CAP CER 1nF 16V 0603 5%</t>
+  </si>
+  <si>
+    <t>C57</t>
+  </si>
+  <si>
+    <t>C0603X102J4RECAUTO</t>
+  </si>
+  <si>
+    <t>1.2M</t>
+  </si>
+  <si>
+    <t>RES 1200K OHM 1/8W 0.1% 0805</t>
+  </si>
+  <si>
+    <t>R_ESD</t>
+  </si>
+  <si>
+    <t>RG2012P-125-B-T5</t>
+  </si>
+  <si>
+    <t>1.65K</t>
+  </si>
+  <si>
+    <t>RES 1.65K OHM 1/10W 0.1% 0805</t>
+  </si>
+  <si>
+    <t>R27</t>
+  </si>
+  <si>
+    <t>PCF0805R-1K65BT1</t>
+  </si>
+  <si>
+    <t>TT Welwyn</t>
+  </si>
+  <si>
+    <t>3.24k 1/8W</t>
+  </si>
+  <si>
+    <t>RES 3.24k OHM 1/8W 1% 0805 SMD</t>
+  </si>
+  <si>
+    <t>R59</t>
+  </si>
+  <si>
+    <t>CRCW08053K24FKEA</t>
+  </si>
+  <si>
+    <t>4K7</t>
+  </si>
+  <si>
+    <t>RES 4K7 OHM 1/8W 1% 0603</t>
+  </si>
+  <si>
+    <t>R64</t>
+  </si>
+  <si>
+    <t>MCT06030C4701FP500</t>
+  </si>
+  <si>
+    <t>4.02k</t>
+  </si>
+  <si>
+    <t>RES 4.02k OHM 1/8W 0.1% 0805</t>
+  </si>
+  <si>
+    <t>R36</t>
+  </si>
+  <si>
+    <t>ERA-6AEB4021V</t>
+  </si>
+  <si>
+    <t>10uH/6.4A/51.8mOHM</t>
+  </si>
+  <si>
+    <t>INDUCTOR 2.2UH 6.4A SMD</t>
+  </si>
+  <si>
+    <t>L6</t>
+  </si>
+  <si>
+    <t>IHLP3232DZER100M11</t>
+  </si>
+  <si>
+    <t>Ind_IHLP</t>
+  </si>
+  <si>
+    <t>Vishay Dale</t>
+  </si>
+  <si>
+    <t>27uH/4.3A/42.5mOHM</t>
+  </si>
+  <si>
+    <t>INDUCTOR 27UH 4.3A SMD</t>
+  </si>
+  <si>
+    <t>L3</t>
+  </si>
+  <si>
+    <t>7447798271</t>
+  </si>
+  <si>
+    <t>30R@100Mhz, 3A</t>
+  </si>
+  <si>
+    <t>Ferrite Bead 30 OHM 3A 100MHz</t>
+  </si>
+  <si>
+    <t>FB1</t>
+  </si>
+  <si>
+    <t>BLM21PG300SN1D</t>
+  </si>
+  <si>
+    <t>IND0805</t>
+  </si>
+  <si>
+    <t>32MHz 10ppm</t>
+  </si>
+  <si>
+    <t>32MHz ±10ppm Crystal 10pF 60 Ohm -40°C ~ 125°C</t>
+  </si>
+  <si>
+    <t>Y1</t>
+  </si>
+  <si>
+    <t>ABM8X-102-32.000MHZ-T</t>
+  </si>
+  <si>
+    <t>XTAL_ABM8X</t>
+  </si>
+  <si>
+    <t>Abracon</t>
+  </si>
+  <si>
+    <t>32.768kHz 12.5pF</t>
+  </si>
+  <si>
+    <t>32.768kHz ±20ppm Crystal 12.5pF 70 kOhm -40°C ~ 125°C</t>
+  </si>
+  <si>
+    <t>Y2</t>
+  </si>
+  <si>
+    <t>ECS-.327-12.5-34S-TR</t>
+  </si>
+  <si>
+    <t>ABS06 0805</t>
+  </si>
+  <si>
+    <t>ECS International</t>
+  </si>
+  <si>
     <t>47k</t>
-  </si>
-  <si>
-    <t>RES 47k OHM 1/10W 1% 0805</t>
-  </si>
-  <si>
-    <t>V1, V2, V3, V4</t>
-  </si>
-  <si>
-    <t>RC0805FR-0747KL</t>
-  </si>
-  <si>
-    <t>150R</t>
-  </si>
-  <si>
-    <t>RES 150R OHM 1/10W 1% 0603</t>
-  </si>
-  <si>
-    <t>R33, R42, R44, R92</t>
-  </si>
-  <si>
-    <t>CRCW0603150RFKEA</t>
-  </si>
-  <si>
-    <t>220uF/6.3V</t>
-  </si>
-  <si>
-    <t>CAP Tantalum 220uF 6.3V 20% 1210</t>
-  </si>
-  <si>
-    <t>C24, C31, C49, C56</t>
-  </si>
-  <si>
-    <t>6TPE220MAZB</t>
-  </si>
-  <si>
-    <t>cc1210</t>
-  </si>
-  <si>
-    <t>Panasonic</t>
-  </si>
-  <si>
-    <t>MOSFET-P-SI4403CDY-T1-GE3</t>
-  </si>
-  <si>
-    <t>MOSFET 1.8V P-Channel 20 V, 0.0155 Ω typ., 13.4 A</t>
-  </si>
-  <si>
-    <t>Q3, Q4, Q5, Q6</t>
-  </si>
-  <si>
-    <t>SI4403CDY-T1-GE3</t>
-  </si>
-  <si>
-    <t>5K9</t>
-  </si>
-  <si>
-    <t>RES 5K9 OHM 1/8W 1% 0805</t>
-  </si>
-  <si>
-    <t>R19, R24, R54</t>
-  </si>
-  <si>
-    <t>71-CRCW0805-5.9K-E3</t>
-  </si>
-  <si>
-    <t>CRCW08055K90FKEA</t>
-  </si>
-  <si>
-    <t>93K1</t>
-  </si>
-  <si>
-    <t>RES 93.1K OHM 1/10W 1% 0603</t>
-  </si>
-  <si>
-    <t>R69, R74, R81</t>
-  </si>
-  <si>
-    <t>CRCW060393K1FKEA</t>
-  </si>
-  <si>
-    <t>100uH/2.2/150.2mOHM</t>
-  </si>
-  <si>
-    <t>MSS1278T-104MLD - 100uH / 2.2A / 150.2mOHM</t>
-  </si>
-  <si>
-    <t>L7, L8, L9</t>
-  </si>
-  <si>
-    <t>IND_HC9</t>
-  </si>
-  <si>
-    <t>0532610671</t>
-  </si>
-  <si>
-    <t>PicoBlade 6 Position Right Angle Connector Header Surface Mount  0.049" (1.25mm)</t>
-  </si>
-  <si>
-    <t>SBW, SW1, SW2</t>
-  </si>
-  <si>
-    <t>53398-0671</t>
-  </si>
-  <si>
-    <t>PICOBLADE 6PIN Right Angle</t>
-  </si>
-  <si>
-    <t>0532610871</t>
-  </si>
-  <si>
-    <t>PicoBlade 8 Position Right Angle Connector Header Surface Mount 0.049" (1.25mm)</t>
-  </si>
-  <si>
-    <t>P8, RTD1, RTD2</t>
-  </si>
-  <si>
-    <t>53261-0871</t>
-  </si>
-  <si>
-    <t>PICOBLADE 8PIN RIGHT ANGLE</t>
-  </si>
-  <si>
-    <t>0.47uF/50V</t>
-  </si>
-  <si>
-    <t>CAP CER 0.47UF 50V 10% X7R 0603</t>
-  </si>
-  <si>
-    <t>C39, C65</t>
-  </si>
-  <si>
-    <t>C1608X7R1H474K080AE</t>
-  </si>
-  <si>
-    <t>TDK</t>
-  </si>
-  <si>
-    <t>RES SMD 1K OHM 1% 1/8W 0805</t>
-  </si>
-  <si>
-    <t>R25, R26</t>
-  </si>
-  <si>
-    <t>ERJ-6ENF1001V</t>
-  </si>
-  <si>
-    <t>2.2uH/9A 15mOHM</t>
-  </si>
-  <si>
-    <t>INDUCTOR 2.2UH 9A SMD</t>
-  </si>
-  <si>
-    <t>L1, L2</t>
-  </si>
-  <si>
-    <t>SRP6540-2R2M</t>
-  </si>
-  <si>
-    <t>Ind_SRP6540</t>
-  </si>
-  <si>
-    <t>Bourns</t>
-  </si>
-  <si>
-    <t>3SMAJ5919B-TP</t>
-  </si>
-  <si>
-    <t>DIODE ZENER 5.6V 3W DO214AC</t>
-  </si>
-  <si>
-    <t>D5, D6</t>
-  </si>
-  <si>
-    <t>MCC</t>
-  </si>
-  <si>
-    <t>5.6nF/100V</t>
-  </si>
-  <si>
-    <t>CAP CER 5.6nF 100V 0603</t>
-  </si>
-  <si>
-    <t>C10, C20</t>
-  </si>
-  <si>
-    <t>C1608C0G2A562J080AE</t>
-  </si>
-  <si>
-    <t>10pF/100V</t>
-  </si>
-  <si>
-    <t>CAP CER 10pF 100V 0805</t>
-  </si>
-  <si>
-    <t>C68, C70</t>
-  </si>
-  <si>
-    <t>08051A100FAT2A</t>
-  </si>
-  <si>
-    <t>11.5k</t>
-  </si>
-  <si>
-    <t>RES 11.5k OHM 1/8W 1% 0805</t>
-  </si>
-  <si>
-    <t>R6, R13</t>
-  </si>
-  <si>
-    <t>AC0805FR-0711K5L</t>
-  </si>
-  <si>
-    <t>12pF/50V</t>
-  </si>
-  <si>
-    <t>CAP CER 12pF 50V 0603</t>
-  </si>
-  <si>
-    <t>C67, C69</t>
-  </si>
-  <si>
-    <t>GQM1885C1H120GB01D</t>
-  </si>
-  <si>
-    <t>13pF/50V</t>
-  </si>
-  <si>
-    <t>CAP CER 13PF 50V 0603 NP0</t>
-  </si>
-  <si>
-    <t>C9, C19</t>
-  </si>
-  <si>
-    <t>C0603C130J5GAC7867</t>
-  </si>
-  <si>
-    <t>KEMET</t>
-  </si>
-  <si>
-    <t>C0603C130J5GACTU</t>
-  </si>
-  <si>
-    <t>16uH/5A/34.5mOHM</t>
-  </si>
-  <si>
-    <t>INDUCTOR 16UH 5A SMD</t>
-  </si>
-  <si>
-    <t>L4, L5</t>
-  </si>
-  <si>
-    <t>7443251600</t>
-  </si>
-  <si>
-    <t>IND_744325xxx</t>
-  </si>
-  <si>
-    <t>19.6k</t>
-  </si>
-  <si>
-    <t>RES 19.6k OHM 1/10W 1% 0603</t>
-  </si>
-  <si>
-    <t>R5, R12</t>
-  </si>
-  <si>
-    <t>ERJ-3EKF1962V</t>
-  </si>
-  <si>
-    <t>30R@100Mhz, 10A</t>
-  </si>
-  <si>
-    <t>Ferrite Bead 30 OHM 10A 100MHz</t>
-  </si>
-  <si>
-    <t>FB3, FB4</t>
-  </si>
-  <si>
-    <t>BLE32PN300SN1L</t>
-  </si>
-  <si>
-    <t>IND1210</t>
-  </si>
-  <si>
-    <t>100K 1/10W</t>
-  </si>
-  <si>
-    <t>RES 100K OHM 1/10W 0.1% 0805</t>
-  </si>
-  <si>
-    <t>R35, R85</t>
-  </si>
-  <si>
-    <t>CPF-A-0805B100KE</t>
-  </si>
-  <si>
-    <t>TE Connectivity</t>
-  </si>
-  <si>
-    <t>140k</t>
-  </si>
-  <si>
-    <t>RES 140k OHM 1/5W 1% 0603</t>
-  </si>
-  <si>
-    <t>R7, R14</t>
-  </si>
-  <si>
-    <t>ERJ-P03F1403V</t>
-  </si>
-  <si>
-    <t>300K</t>
-  </si>
-  <si>
-    <t>RES 300K OHM 1/10W 0.1% 0603</t>
-  </si>
-  <si>
-    <t>R45, R70</t>
-  </si>
-  <si>
-    <t>RG1608P-304-B-T5</t>
-  </si>
-  <si>
-    <t>Susumu</t>
-  </si>
-  <si>
-    <t>1000pF/50V</t>
-  </si>
-  <si>
-    <t>CAP CER 1000pF 50V 10% X7R 0603</t>
-  </si>
-  <si>
-    <t>C37, C38</t>
-  </si>
-  <si>
-    <t>CC0603KRX7R9BB102</t>
-  </si>
-  <si>
-    <t>FSV530AF</t>
-  </si>
-  <si>
-    <t>DIODE SCHOTTKY 30V 5A DO-214AA</t>
-  </si>
-  <si>
-    <t>D1, D2</t>
-  </si>
-  <si>
-    <t>ON Semiconductor / Fairchild</t>
-  </si>
-  <si>
-    <t>Header 5X2IPS1-105-01-S-D</t>
-  </si>
-  <si>
-    <t>10 Position Receptacle Connector 0.100" (2.54mm)</t>
-  </si>
-  <si>
-    <t>P1, P5</t>
-  </si>
-  <si>
-    <t>IPS1-105-01-S-D</t>
-  </si>
-  <si>
-    <t>Samtec</t>
-  </si>
-  <si>
-    <t>Through Hole</t>
-  </si>
-  <si>
-    <t>TPS5420QDRQ1</t>
-  </si>
-  <si>
-    <t>U4, U9</t>
-  </si>
-  <si>
-    <t>SO8 Power PAD</t>
-  </si>
-  <si>
-    <t>TPS54540QDDARQ1</t>
-  </si>
-  <si>
-    <t>U2, U14</t>
-  </si>
-  <si>
-    <t>0.01R/0.5W</t>
-  </si>
-  <si>
-    <t>Current Sense Resistors - SMD 0.01ohm .5% 4 Terminal</t>
-  </si>
-  <si>
-    <t>RSense1</t>
-  </si>
-  <si>
-    <t>LVK12R010DER</t>
-  </si>
-  <si>
-    <t>0.01uF/25V</t>
-  </si>
-  <si>
-    <t>CAP CER 0.01UF 25V 5% X7R 0603</t>
-  </si>
-  <si>
-    <t>C66</t>
-  </si>
-  <si>
-    <t>06033C103JAT4A</t>
-  </si>
-  <si>
-    <t>0.075R/0.5W</t>
-  </si>
-  <si>
-    <t>Current Sense Resistors - SMD 1/2W 0.075 OHMS 1% 4 Terminal</t>
-  </si>
-  <si>
-    <t>Rsense3</t>
-  </si>
-  <si>
-    <t>LVK12R075FER</t>
-  </si>
-  <si>
-    <t>1nF/16V</t>
-  </si>
-  <si>
-    <t>CAP CER 1nF 16V 0603 5%</t>
-  </si>
-  <si>
-    <t>C57</t>
-  </si>
-  <si>
-    <t>C0603X102J4RECAUTO</t>
-  </si>
-  <si>
-    <t>1.2M</t>
-  </si>
-  <si>
-    <t>RES 1200K OHM 1/8W 0.1% 0805</t>
-  </si>
-  <si>
-    <t>R_ESD</t>
-  </si>
-  <si>
-    <t>RG2012P-125-B-T5</t>
-  </si>
-  <si>
-    <t>1.65K</t>
-  </si>
-  <si>
-    <t>RES 1.65K OHM 1/10W 0.1% 0805</t>
-  </si>
-  <si>
-    <t>R27</t>
-  </si>
-  <si>
-    <t>PCF0805R-1K65BT1</t>
-  </si>
-  <si>
-    <t>TT Welwyn</t>
-  </si>
-  <si>
-    <t>3.24k 1/8W</t>
-  </si>
-  <si>
-    <t>RES 3.24k OHM 1/8W 1% 0805 SMD</t>
-  </si>
-  <si>
-    <t>R59</t>
-  </si>
-  <si>
-    <t>CRCW08053K24FKEA</t>
-  </si>
-  <si>
-    <t>4K7</t>
-  </si>
-  <si>
-    <t>RES 4K7 OHM 1/8W 1% 0603</t>
-  </si>
-  <si>
-    <t>R64</t>
-  </si>
-  <si>
-    <t>MCT06030C4701FP500</t>
-  </si>
-  <si>
-    <t>4.02k</t>
-  </si>
-  <si>
-    <t>RES 4.02k OHM 1/8W 0.1% 0805</t>
-  </si>
-  <si>
-    <t>R36</t>
-  </si>
-  <si>
-    <t>ERA-6AEB4021V</t>
-  </si>
-  <si>
-    <t>10uH/6.4A/51.8mOHM</t>
-  </si>
-  <si>
-    <t>INDUCTOR 2.2UH 6.4A SMD</t>
-  </si>
-  <si>
-    <t>L6</t>
-  </si>
-  <si>
-    <t>IHLP3232DZER100M11</t>
-  </si>
-  <si>
-    <t>Ind_IHLP</t>
-  </si>
-  <si>
-    <t>Vishay Dale</t>
-  </si>
-  <si>
-    <t>27uH/4.3A/42.5mOHM</t>
-  </si>
-  <si>
-    <t>INDUCTOR 27UH 4.3A SMD</t>
-  </si>
-  <si>
-    <t>L3</t>
-  </si>
-  <si>
-    <t>7447798271</t>
-  </si>
-  <si>
-    <t>30R@100Mhz, 3A</t>
-  </si>
-  <si>
-    <t>Ferrite Bead 30 OHM 3A 100MHz</t>
-  </si>
-  <si>
-    <t>FB1</t>
-  </si>
-  <si>
-    <t>BLM21PG300SN1D</t>
-  </si>
-  <si>
-    <t>IND0805</t>
-  </si>
-  <si>
-    <t>32MHz 10ppm</t>
-  </si>
-  <si>
-    <t>32MHz ±10ppm Crystal 10pF 60 Ohm -40°C ~ 125°C</t>
-  </si>
-  <si>
-    <t>Y1</t>
-  </si>
-  <si>
-    <t>ABM8X-102-32.000MHZ-T</t>
-  </si>
-  <si>
-    <t>XTAL_ABM8X</t>
-  </si>
-  <si>
-    <t>Abracon</t>
-  </si>
-  <si>
-    <t>32.768kHz 12.5pF</t>
-  </si>
-  <si>
-    <t>32.768kHz ±20ppm Crystal 12.5pF 70 kOhm -40°C ~ 125°C</t>
-  </si>
-  <si>
-    <t>Y2</t>
-  </si>
-  <si>
-    <t>ECS-.327-12.5-34S-TR</t>
-  </si>
-  <si>
-    <t>ABS06 0805</t>
-  </si>
-  <si>
-    <t>ECS International</t>
   </si>
   <si>
     <t>RES 47K OHM 1/8W 0.5% 0603</t>
@@ -1510,12 +1516,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" baseColWidth="0"/>
   <cols>
-    <col min="1" max="1" width="21.515625" customWidth="1"/>
-    <col min="2" max="2" width="14.52734375" customWidth="1"/>
-    <col min="3" max="3" width="15.9921875" customWidth="1"/>
-    <col min="4" max="4" width="17.77734375" customWidth="1"/>
-    <col min="5" max="5" width="41.50390625" customWidth="1"/>
-    <col min="6" max="10" width="16.8046875" customWidth="1"/>
+    <col min="1" max="1" width="21.671875" customWidth="1"/>
+    <col min="2" max="2" width="14.68359375" customWidth="1"/>
+    <col min="3" max="3" width="16.1484375" customWidth="1"/>
+    <col min="4" max="4" width="17.93359375" customWidth="1"/>
+    <col min="5" max="5" width="41.66015625" customWidth="1"/>
+    <col min="6" max="10" width="16.9609375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10">
@@ -2643,16 +2649,16 @@
         <v>5</v>
       </c>
       <c r="F37" s="16" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G37" s="16" t="s">
         <v>104</v>
       </c>
       <c r="H37" s="16" t="s">
+        <v>188</v>
+      </c>
+      <c r="I37" s="16" t="s">
         <v>187</v>
-      </c>
-      <c r="I37" s="16" t="s">
-        <v>184</v>
       </c>
       <c r="J37" s="16" t="s">
         <v>17</v>
@@ -2660,22 +2666,22 @@
     </row>
     <row r="38" spans="1:10">
       <c r="A38" s="28" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B38" s="16" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C38" s="17">
         <v>2</v>
       </c>
       <c r="D38" s="16" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="E38" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F38" s="16" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="G38" s="16" t="s">
         <v>15</v>
@@ -2684,28 +2690,28 @@
         <v>174</v>
       </c>
       <c r="I38" s="16" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="J38" s="16"/>
     </row>
     <row r="39" spans="1:10">
       <c r="A39" s="28" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B39" s="16" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C39" s="17">
         <v>2</v>
       </c>
       <c r="D39" s="16" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="E39" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F39" s="16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="G39" s="16" t="s">
         <v>21</v>
@@ -2714,7 +2720,7 @@
         <v>64</v>
       </c>
       <c r="I39" s="16" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="J39" s="16" t="s">
         <v>17</v>
@@ -2722,22 +2728,22 @@
     </row>
     <row r="40" spans="1:10">
       <c r="A40" s="28" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B40" s="16" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C40" s="17">
         <v>2</v>
       </c>
       <c r="D40" s="16" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="E40" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F40" s="16" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="G40" s="16" t="s">
         <v>37</v>
@@ -2746,28 +2752,28 @@
         <v>16</v>
       </c>
       <c r="I40" s="16" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="J40" s="16"/>
     </row>
     <row r="41" spans="1:10">
       <c r="A41" s="28" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="C41" s="17">
         <v>2</v>
       </c>
       <c r="D41" s="16" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="E41" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F41" s="16" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="G41" s="16" t="s">
         <v>15</v>
@@ -2776,7 +2782,7 @@
         <v>47</v>
       </c>
       <c r="I41" s="16" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
       <c r="J41" s="16" t="s">
         <v>17</v>
@@ -2784,31 +2790,31 @@
     </row>
     <row r="42" spans="1:10">
       <c r="A42" s="28" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B42" s="16" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C42" s="17">
         <v>2</v>
       </c>
       <c r="D42" s="16" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
       <c r="E42" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F42" s="16" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="G42" s="16" t="s">
         <v>15</v>
       </c>
       <c r="H42" s="16" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I42" s="16" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="J42" s="16" t="s">
         <v>17</v>
@@ -2816,31 +2822,31 @@
     </row>
     <row r="43" spans="1:10">
       <c r="A43" s="28" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="B43" s="16" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="C43" s="17">
         <v>2</v>
       </c>
       <c r="D43" s="16" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="E43" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F43" s="16" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G43" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H43" s="16" t="s">
         <v>58</v>
       </c>
       <c r="I43" s="16" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="J43" s="16" t="s">
         <v>17</v>
@@ -2848,22 +2854,22 @@
     </row>
     <row r="44" spans="1:10">
       <c r="A44" s="28" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="B44" s="16" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="C44" s="17">
         <v>2</v>
       </c>
       <c r="D44" s="16" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="E44" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F44" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G44" s="16" t="s">
         <v>99</v>
@@ -2872,7 +2878,7 @@
         <v>142</v>
       </c>
       <c r="I44" s="16" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="J44" s="16" t="s">
         <v>17</v>
@@ -2880,31 +2886,31 @@
     </row>
     <row r="45" spans="1:10">
       <c r="A45" s="28" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="B45" s="16" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="C45" s="17">
         <v>2</v>
       </c>
       <c r="D45" s="16" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="E45" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F45" s="16" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="G45" s="16" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="H45" s="16" t="s">
         <v>47</v>
       </c>
       <c r="I45" s="16" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="J45" s="16" t="s">
         <v>17</v>
@@ -2912,52 +2918,52 @@
     </row>
     <row r="46" spans="1:10">
       <c r="A46" s="28" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
       <c r="B46" s="16" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="C46" s="17">
         <v>2</v>
       </c>
       <c r="D46" s="16" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="E46" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F46" s="16" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="G46" s="16" t="s">
         <v>37</v>
       </c>
       <c r="H46" s="16" t="s">
+        <v>229</v>
+      </c>
+      <c r="I46" s="16" t="s">
         <v>228</v>
-      </c>
-      <c r="I46" s="16" t="s">
-        <v>227</v>
       </c>
       <c r="J46" s="16"/>
     </row>
     <row r="47" spans="1:10">
       <c r="A47" s="28" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="B47" s="16" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="C47" s="17">
         <v>2</v>
       </c>
       <c r="D47" s="16" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="E47" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F47" s="16" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="G47" s="16" t="s">
         <v>99</v>
@@ -2966,7 +2972,7 @@
         <v>142</v>
       </c>
       <c r="I47" s="16" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
       <c r="J47" s="16" t="s">
         <v>17</v>
@@ -2974,52 +2980,52 @@
     </row>
     <row r="48" spans="1:10">
       <c r="A48" s="28" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B48" s="16" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C48" s="17">
         <v>2</v>
       </c>
       <c r="D48" s="16" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
       <c r="E48" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F48" s="16" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="G48" s="16" t="s">
         <v>99</v>
       </c>
       <c r="H48" s="16" t="s">
+        <v>238</v>
+      </c>
+      <c r="I48" s="16" t="s">
         <v>237</v>
-      </c>
-      <c r="I48" s="16" t="s">
-        <v>236</v>
       </c>
       <c r="J48" s="16"/>
     </row>
     <row r="49" spans="1:10">
       <c r="A49" s="28" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="B49" s="16" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="C49" s="17">
         <v>2</v>
       </c>
       <c r="D49" s="16" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="E49" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F49" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="G49" s="16" t="s">
         <v>15</v>
@@ -3028,7 +3034,7 @@
         <v>16</v>
       </c>
       <c r="I49" s="16" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="J49" s="16" t="s">
         <v>17</v>
@@ -3036,31 +3042,31 @@
     </row>
     <row r="50" spans="1:10">
       <c r="A50" s="28" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B50" s="16" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="C50" s="17">
         <v>2</v>
       </c>
       <c r="D50" s="16" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="E50" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F50" s="16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="G50" s="16" t="s">
         <v>104</v>
       </c>
       <c r="H50" s="16" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I50" s="16" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="J50" s="16" t="s">
         <v>17</v>
@@ -3068,63 +3074,63 @@
     </row>
     <row r="51" spans="1:10">
       <c r="A51" s="28" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B51" s="16" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C51" s="17">
         <v>2</v>
       </c>
       <c r="D51" s="16" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="E51" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F51" s="16" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="G51" s="16" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="H51" s="16" t="s">
+        <v>251</v>
+      </c>
+      <c r="I51" s="16" t="s">
         <v>250</v>
       </c>
-      <c r="I51" s="16" t="s">
-        <v>249</v>
-      </c>
       <c r="J51" s="16" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="52" spans="1:10">
       <c r="A52" s="28" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="B52" s="16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="C52" s="17">
         <v>2</v>
       </c>
       <c r="D52" s="16" t="s">
+        <v>254</v>
+      </c>
+      <c r="E52" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F52" s="16" t="s">
         <v>253</v>
       </c>
-      <c r="E52" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F52" s="16" t="s">
-        <v>252</v>
-      </c>
       <c r="G52" s="16" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H52" s="16" t="s">
         <v>115</v>
       </c>
       <c r="I52" s="16" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="J52" s="16" t="s">
         <v>17</v>
@@ -3132,31 +3138,31 @@
     </row>
     <row r="53" spans="1:10">
       <c r="A53" s="28" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B53" s="16" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="C53" s="17">
         <v>2</v>
       </c>
       <c r="D53" s="16" t="s">
+        <v>257</v>
+      </c>
+      <c r="E53" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F53" s="16" t="s">
         <v>256</v>
       </c>
-      <c r="E53" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F53" s="16" t="s">
+      <c r="G53" s="16" t="s">
         <v>255</v>
-      </c>
-      <c r="G53" s="16" t="s">
-        <v>254</v>
       </c>
       <c r="H53" s="16" t="s">
         <v>115</v>
       </c>
       <c r="I53" s="16" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="J53" s="16" t="s">
         <v>17</v>
@@ -3164,22 +3170,22 @@
     </row>
     <row r="54" spans="1:10">
       <c r="A54" s="28" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="B54" s="16" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="C54" s="17">
         <v>1</v>
       </c>
       <c r="D54" s="16" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="E54" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F54" s="16" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="G54" s="16" t="s">
         <v>83</v>
@@ -3188,7 +3194,7 @@
         <v>84</v>
       </c>
       <c r="I54" s="16" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="J54" s="16" t="s">
         <v>17</v>
@@ -3196,22 +3202,22 @@
     </row>
     <row r="55" spans="1:10">
       <c r="A55" s="28" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B55" s="16" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C55" s="17">
         <v>1</v>
       </c>
       <c r="D55" s="16" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="E55" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F55" s="16" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="G55" s="16" t="s">
         <v>15</v>
@@ -3220,7 +3226,7 @@
         <v>64</v>
       </c>
       <c r="I55" s="16" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="J55" s="16" t="s">
         <v>17</v>
@@ -3228,22 +3234,22 @@
     </row>
     <row r="56" spans="1:10">
       <c r="A56" s="28" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B56" s="16" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C56" s="17">
         <v>1</v>
       </c>
       <c r="D56" s="16" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E56" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F56" s="16" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G56" s="16" t="s">
         <v>83</v>
@@ -3252,37 +3258,37 @@
         <v>84</v>
       </c>
       <c r="I56" s="16" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="J56" s="16"/>
     </row>
     <row r="57" spans="1:10">
       <c r="A57" s="28" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="B57" s="16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="C57" s="17">
         <v>1</v>
       </c>
       <c r="D57" s="16" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="E57" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F57" s="16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="G57" s="16" t="s">
         <v>21</v>
       </c>
       <c r="H57" s="16" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="I57" s="16" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="J57" s="16" t="s">
         <v>17</v>
@@ -3290,82 +3296,82 @@
     </row>
     <row r="58" spans="1:10">
       <c r="A58" s="28" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="B58" s="16" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="C58" s="17">
         <v>1</v>
       </c>
       <c r="D58" s="16" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E58" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F58" s="16" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="G58" s="16" t="s">
         <v>37</v>
       </c>
       <c r="H58" s="16" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="I58" s="16" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="J58" s="16"/>
     </row>
     <row r="59" spans="1:10">
       <c r="A59" s="28" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="C59" s="17">
         <v>1</v>
       </c>
       <c r="D59" s="16" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="E59" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F59" s="16" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="G59" s="16" t="s">
         <v>37</v>
       </c>
       <c r="H59" s="16" t="s">
+        <v>282</v>
+      </c>
+      <c r="I59" s="16" t="s">
         <v>281</v>
-      </c>
-      <c r="I59" s="16" t="s">
-        <v>280</v>
       </c>
       <c r="J59" s="16"/>
     </row>
     <row r="60" spans="1:10">
       <c r="A60" s="28" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B60" s="16" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="C60" s="17">
         <v>1</v>
       </c>
       <c r="D60" s="16" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="E60" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F60" s="16" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="G60" s="16" t="s">
         <v>37</v>
@@ -3374,28 +3380,28 @@
         <v>33</v>
       </c>
       <c r="I60" s="16" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="J60" s="16"/>
     </row>
     <row r="61" spans="1:10">
       <c r="A61" s="28" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B61" s="16" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C61" s="17">
         <v>1</v>
       </c>
       <c r="D61" s="16" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="E61" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F61" s="16" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="G61" s="16" t="s">
         <v>99</v>
@@ -3404,7 +3410,7 @@
         <v>121</v>
       </c>
       <c r="I61" s="16" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="J61" s="16" t="s">
         <v>17</v>
@@ -3412,22 +3418,22 @@
     </row>
     <row r="62" spans="1:10">
       <c r="A62" s="28" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="B62" s="16" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="C62" s="17">
         <v>1</v>
       </c>
       <c r="D62" s="16" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="E62" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F62" s="16" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="G62" s="16" t="s">
         <v>37</v>
@@ -3436,7 +3442,7 @@
         <v>142</v>
       </c>
       <c r="I62" s="16" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="J62" s="16" t="s">
         <v>17</v>
@@ -3444,31 +3450,31 @@
     </row>
     <row r="63" spans="1:10">
       <c r="A63" s="28" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B63" s="16" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C63" s="17">
         <v>1</v>
       </c>
       <c r="D63" s="16" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="E63" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F63" s="16" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="G63" s="16" t="s">
+        <v>299</v>
+      </c>
+      <c r="H63" s="16" t="s">
+        <v>300</v>
+      </c>
+      <c r="I63" s="16" t="s">
         <v>298</v>
-      </c>
-      <c r="H63" s="16" t="s">
-        <v>299</v>
-      </c>
-      <c r="I63" s="16" t="s">
-        <v>297</v>
       </c>
       <c r="J63" s="16" t="s">
         <v>17</v>
@@ -3476,31 +3482,31 @@
     </row>
     <row r="64" spans="1:10">
       <c r="A64" s="28" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="B64" s="16" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="C64" s="17">
         <v>1</v>
       </c>
       <c r="D64" s="16" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="E64" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F64" s="16" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="G64" s="16" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="H64" s="16" t="s">
         <v>58</v>
       </c>
       <c r="I64" s="16" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="J64" s="16" t="s">
         <v>17</v>
@@ -3508,61 +3514,61 @@
     </row>
     <row r="65" spans="1:10">
       <c r="A65" s="28" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B65" s="16" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="C65" s="17">
         <v>1</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="E65" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F65" s="16" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="G65" s="16" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="H65" s="16" t="s">
         <v>47</v>
       </c>
       <c r="I65" s="16" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="J65" s="16"/>
     </row>
     <row r="66" spans="1:10">
       <c r="A66" s="28" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B66" s="16" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C66" s="17">
         <v>1</v>
       </c>
       <c r="D66" s="16" t="s">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="E66" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F66" s="16" t="s">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="G66" s="16" t="s">
+        <v>314</v>
+      </c>
+      <c r="H66" s="16" t="s">
+        <v>315</v>
+      </c>
+      <c r="I66" s="16" t="s">
         <v>313</v>
-      </c>
-      <c r="H66" s="16" t="s">
-        <v>314</v>
-      </c>
-      <c r="I66" s="16" t="s">
-        <v>312</v>
       </c>
       <c r="J66" s="16" t="s">
         <v>17</v>
@@ -3570,31 +3576,31 @@
     </row>
     <row r="67" spans="1:10">
       <c r="A67" s="28" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="B67" s="16" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C67" s="17">
         <v>1</v>
       </c>
       <c r="D67" s="16" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="E67" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F67" s="16" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="G67" s="16" t="s">
+        <v>320</v>
+      </c>
+      <c r="H67" s="16" t="s">
+        <v>321</v>
+      </c>
+      <c r="I67" s="16" t="s">
         <v>319</v>
-      </c>
-      <c r="H67" s="16" t="s">
-        <v>320</v>
-      </c>
-      <c r="I67" s="16" t="s">
-        <v>318</v>
       </c>
       <c r="J67" s="16" t="s">
         <v>17</v>
@@ -3602,22 +3608,22 @@
     </row>
     <row r="68" spans="1:10">
       <c r="A68" s="28" t="s">
-        <v>129</v>
+        <v>322</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>321</v>
+        <v>323</v>
       </c>
       <c r="C68" s="17">
         <v>1</v>
       </c>
       <c r="D68" s="16" t="s">
-        <v>322</v>
+        <v>324</v>
       </c>
       <c r="E68" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F68" s="16" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="G68" s="16" t="s">
         <v>99</v>
@@ -3626,28 +3632,28 @@
         <v>33</v>
       </c>
       <c r="I68" s="16" t="s">
-        <v>323</v>
+        <v>325</v>
       </c>
       <c r="J68" s="16"/>
     </row>
     <row r="69" spans="1:10">
       <c r="A69" s="28" t="s">
-        <v>324</v>
+        <v>326</v>
       </c>
       <c r="B69" s="16" t="s">
-        <v>325</v>
+        <v>327</v>
       </c>
       <c r="C69" s="17">
         <v>1</v>
       </c>
       <c r="D69" s="16" t="s">
-        <v>326</v>
+        <v>328</v>
       </c>
       <c r="E69" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F69" s="16" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="G69" s="16" t="s">
         <v>37</v>
@@ -3656,7 +3662,7 @@
         <v>142</v>
       </c>
       <c r="I69" s="16" t="s">
-        <v>327</v>
+        <v>329</v>
       </c>
       <c r="J69" s="16" t="s">
         <v>17</v>
@@ -3664,22 +3670,22 @@
     </row>
     <row r="70" spans="1:10">
       <c r="A70" s="28" t="s">
-        <v>328</v>
+        <v>330</v>
       </c>
       <c r="B70" s="16" t="s">
-        <v>329</v>
+        <v>331</v>
       </c>
       <c r="C70" s="17">
         <v>1</v>
       </c>
       <c r="D70" s="16" t="s">
-        <v>330</v>
+        <v>332</v>
       </c>
       <c r="E70" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F70" s="16" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="G70" s="16" t="s">
         <v>37</v>
@@ -3688,7 +3694,7 @@
         <v>142</v>
       </c>
       <c r="I70" s="16" t="s">
-        <v>331</v>
+        <v>333</v>
       </c>
       <c r="J70" s="16" t="s">
         <v>17</v>
@@ -3696,22 +3702,22 @@
     </row>
     <row r="71" spans="1:10">
       <c r="A71" s="28" t="s">
-        <v>332</v>
+        <v>334</v>
       </c>
       <c r="B71" s="16" t="s">
-        <v>333</v>
+        <v>335</v>
       </c>
       <c r="C71" s="17">
         <v>1</v>
       </c>
       <c r="D71" s="16" t="s">
-        <v>334</v>
+        <v>336</v>
       </c>
       <c r="E71" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F71" s="16" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="G71" s="16" t="s">
         <v>99</v>
@@ -3720,31 +3726,31 @@
         <v>121</v>
       </c>
       <c r="I71" s="16" t="s">
-        <v>335</v>
+        <v>337</v>
       </c>
       <c r="J71" s="16"/>
     </row>
     <row r="72" spans="1:10">
       <c r="A72" s="28" t="s">
-        <v>336</v>
+        <v>338</v>
       </c>
       <c r="B72" s="16" t="s">
-        <v>337</v>
+        <v>339</v>
       </c>
       <c r="C72" s="17">
         <v>1</v>
       </c>
       <c r="D72" s="16" t="s">
+        <v>340</v>
+      </c>
+      <c r="E72" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F72" s="16" t="s">
         <v>338</v>
       </c>
-      <c r="E72" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F72" s="16" t="s">
-        <v>336</v>
-      </c>
       <c r="G72" s="16" t="s">
-        <v>339</v>
+        <v>341</v>
       </c>
       <c r="H72" s="16"/>
       <c r="I72" s="16"/>
@@ -3752,25 +3758,25 @@
     </row>
     <row r="73" spans="1:10">
       <c r="A73" s="28" t="s">
-        <v>340</v>
+        <v>342</v>
       </c>
       <c r="B73" s="16" t="s">
-        <v>341</v>
+        <v>343</v>
       </c>
       <c r="C73" s="17">
         <v>1</v>
       </c>
       <c r="D73" s="16" t="s">
+        <v>344</v>
+      </c>
+      <c r="E73" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F73" s="16" t="s">
         <v>342</v>
       </c>
-      <c r="E73" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F73" s="16" t="s">
-        <v>340</v>
-      </c>
       <c r="G73" s="16" t="s">
-        <v>343</v>
+        <v>345</v>
       </c>
       <c r="H73" s="16"/>
       <c r="I73" s="16"/>
@@ -3778,31 +3784,31 @@
     </row>
     <row r="74" spans="1:10">
       <c r="A74" s="28" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="B74" s="16" t="s">
-        <v>345</v>
+        <v>347</v>
       </c>
       <c r="C74" s="17">
         <v>1</v>
       </c>
       <c r="D74" s="16" t="s">
+        <v>348</v>
+      </c>
+      <c r="E74" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F74" s="16" t="s">
         <v>346</v>
       </c>
-      <c r="E74" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F74" s="16" t="s">
-        <v>344</v>
-      </c>
       <c r="G74" s="16" t="s">
-        <v>347</v>
+        <v>349</v>
       </c>
       <c r="H74" s="16" t="s">
         <v>70</v>
       </c>
       <c r="I74" s="16" t="s">
-        <v>344</v>
+        <v>346</v>
       </c>
       <c r="J74" s="16" t="s">
         <v>17</v>
@@ -3810,61 +3816,61 @@
     </row>
     <row r="75" spans="1:10">
       <c r="A75" s="28" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="B75" s="16" t="s">
-        <v>349</v>
+        <v>351</v>
       </c>
       <c r="C75" s="17">
         <v>1</v>
       </c>
       <c r="D75" s="16" t="s">
-        <v>350</v>
+        <v>352</v>
       </c>
       <c r="E75" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F75" s="16" t="s">
-        <v>351</v>
+        <v>353</v>
       </c>
       <c r="G75" s="16" t="s">
-        <v>352</v>
+        <v>354</v>
       </c>
       <c r="H75" s="16" t="s">
         <v>115</v>
       </c>
       <c r="I75" s="16" t="s">
-        <v>348</v>
+        <v>350</v>
       </c>
       <c r="J75" s="16"/>
     </row>
     <row r="76" spans="1:10">
       <c r="A76" s="28" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="B76" s="16" t="s">
-        <v>354</v>
+        <v>356</v>
       </c>
       <c r="C76" s="17">
         <v>1</v>
       </c>
       <c r="D76" s="16" t="s">
+        <v>357</v>
+      </c>
+      <c r="E76" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F76" s="16" t="s">
         <v>355</v>
       </c>
-      <c r="E76" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F76" s="16" t="s">
-        <v>353</v>
-      </c>
       <c r="G76" s="16" t="s">
-        <v>356</v>
+        <v>358</v>
       </c>
       <c r="H76" s="16" t="s">
         <v>105</v>
       </c>
       <c r="I76" s="16" t="s">
-        <v>353</v>
+        <v>355</v>
       </c>
       <c r="J76" s="16" t="s">
         <v>17</v>
@@ -3872,31 +3878,31 @@
     </row>
     <row r="77" spans="1:10">
       <c r="A77" s="28" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="B77" s="16" t="s">
-        <v>358</v>
+        <v>360</v>
       </c>
       <c r="C77" s="17">
         <v>1</v>
       </c>
       <c r="D77" s="16" t="s">
+        <v>361</v>
+      </c>
+      <c r="E77" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F77" s="16" t="s">
         <v>359</v>
       </c>
-      <c r="E77" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F77" s="16" t="s">
-        <v>357</v>
-      </c>
       <c r="G77" s="16" t="s">
-        <v>360</v>
+        <v>362</v>
       </c>
       <c r="H77" s="16" t="s">
-        <v>361</v>
+        <v>363</v>
       </c>
       <c r="I77" s="16" t="s">
-        <v>357</v>
+        <v>359</v>
       </c>
       <c r="J77" s="16" t="s">
         <v>17</v>
@@ -3907,28 +3913,28 @@
         <v>53</v>
       </c>
       <c r="B78" s="16" t="s">
-        <v>362</v>
+        <v>364</v>
       </c>
       <c r="C78" s="17">
         <v>1</v>
       </c>
       <c r="D78" s="16" t="s">
-        <v>363</v>
+        <v>365</v>
       </c>
       <c r="E78" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F78" s="16" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="G78" s="16" t="s">
         <v>94</v>
       </c>
       <c r="H78" s="16" t="s">
-        <v>365</v>
+        <v>367</v>
       </c>
       <c r="I78" s="16" t="s">
-        <v>364</v>
+        <v>366</v>
       </c>
       <c r="J78" s="16"/>
     </row>
@@ -3937,60 +3943,60 @@
         <v>53</v>
       </c>
       <c r="B79" s="16" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="C79" s="17">
         <v>1</v>
       </c>
       <c r="D79" s="16" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="E79" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F79" s="16" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
       <c r="G79" s="16" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="H79" s="16" t="s">
+        <v>372</v>
+      </c>
+      <c r="I79" s="16" t="s">
         <v>370</v>
       </c>
-      <c r="I79" s="16" t="s">
-        <v>368</v>
-      </c>
       <c r="J79" s="16" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="80" spans="1:10">
       <c r="A80" s="28" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="B80" s="16" t="s">
-        <v>372</v>
+        <v>374</v>
       </c>
       <c r="C80" s="17">
         <v>1</v>
       </c>
       <c r="D80" s="16" t="s">
+        <v>375</v>
+      </c>
+      <c r="E80" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F80" s="16" t="s">
         <v>373</v>
       </c>
-      <c r="E80" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F80" s="16" t="s">
-        <v>371</v>
-      </c>
       <c r="G80" s="16" t="s">
-        <v>374</v>
+        <v>376</v>
       </c>
       <c r="H80" s="16" t="s">
         <v>74</v>
       </c>
       <c r="I80" s="16" t="s">
-        <v>375</v>
+        <v>377</v>
       </c>
       <c r="J80" s="16" t="s">
         <v>17</v>
@@ -3998,31 +4004,31 @@
     </row>
     <row r="81" spans="1:10">
       <c r="A81" s="28" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="B81" s="16" t="s">
-        <v>377</v>
+        <v>379</v>
       </c>
       <c r="C81" s="17">
         <v>1</v>
       </c>
       <c r="D81" s="16" t="s">
+        <v>380</v>
+      </c>
+      <c r="E81" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F81" s="16" t="s">
         <v>378</v>
       </c>
-      <c r="E81" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F81" s="16" t="s">
-        <v>376</v>
-      </c>
       <c r="G81" s="16" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="H81" s="16" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="I81" s="16" t="s">
-        <v>376</v>
+        <v>378</v>
       </c>
       <c r="J81" s="16" t="s">
         <v>17</v>
@@ -4030,31 +4036,31 @@
     </row>
     <row r="82" spans="1:10">
       <c r="A82" s="28" t="s">
-        <v>380</v>
+        <v>382</v>
       </c>
       <c r="B82" s="16" t="s">
-        <v>381</v>
+        <v>383</v>
       </c>
       <c r="C82" s="17">
         <v>1</v>
       </c>
       <c r="D82" s="16" t="s">
+        <v>384</v>
+      </c>
+      <c r="E82" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F82" s="16" t="s">
         <v>382</v>
       </c>
-      <c r="E82" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F82" s="16" t="s">
-        <v>380</v>
-      </c>
       <c r="G82" s="16" t="s">
-        <v>383</v>
+        <v>385</v>
       </c>
       <c r="H82" s="16" t="s">
         <v>115</v>
       </c>
       <c r="I82" s="16" t="s">
-        <v>384</v>
+        <v>386</v>
       </c>
       <c r="J82" s="16" t="s">
         <v>17</v>
@@ -4062,63 +4068,63 @@
     </row>
     <row r="83" spans="1:10">
       <c r="A83" s="28" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="B83" s="16" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="C83" s="17">
         <v>1</v>
       </c>
       <c r="D83" s="16" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="E83" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F83" s="16" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="G83" s="16" t="s">
-        <v>385</v>
+        <v>387</v>
       </c>
       <c r="H83" s="16" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="I83" s="16" t="s">
-        <v>386</v>
+        <v>388</v>
       </c>
       <c r="J83" s="16" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
     </row>
     <row r="84" spans="1:10">
       <c r="A84" s="28" t="s">
-        <v>387</v>
+        <v>389</v>
       </c>
       <c r="B84" s="16" t="s">
-        <v>388</v>
+        <v>390</v>
       </c>
       <c r="C84" s="17">
         <v>1</v>
       </c>
       <c r="D84" s="16" t="s">
-        <v>389</v>
+        <v>391</v>
       </c>
       <c r="E84" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F84" s="16" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="G84" s="16" t="s">
         <v>57</v>
       </c>
       <c r="H84" s="16" t="s">
-        <v>391</v>
+        <v>393</v>
       </c>
       <c r="I84" s="16" t="s">
-        <v>390</v>
+        <v>392</v>
       </c>
       <c r="J84" s="16" t="s">
         <v>17</v>
@@ -4126,61 +4132,61 @@
     </row>
     <row r="85" spans="1:10">
       <c r="A85" s="28" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="B85" s="16" t="s">
-        <v>393</v>
+        <v>395</v>
       </c>
       <c r="C85" s="17">
         <v>1</v>
       </c>
       <c r="D85" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="E85" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F85" s="16" t="s">
         <v>394</v>
       </c>
-      <c r="E85" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F85" s="16" t="s">
-        <v>392</v>
-      </c>
       <c r="G85" s="16" t="s">
-        <v>395</v>
+        <v>397</v>
       </c>
       <c r="H85" s="16" t="s">
         <v>115</v>
       </c>
       <c r="I85" s="16" t="s">
-        <v>392</v>
+        <v>394</v>
       </c>
       <c r="J85" s="16"/>
     </row>
     <row r="86" spans="1:10">
       <c r="A86" s="28" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="B86" s="16" t="s">
-        <v>397</v>
+        <v>399</v>
       </c>
       <c r="C86" s="17">
         <v>1</v>
       </c>
       <c r="D86" s="16" t="s">
+        <v>400</v>
+      </c>
+      <c r="E86" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="F86" s="16" t="s">
         <v>398</v>
       </c>
-      <c r="E86" s="16" t="s">
-        <v>5</v>
-      </c>
-      <c r="F86" s="16" t="s">
-        <v>396</v>
-      </c>
       <c r="G86" s="16" t="s">
-        <v>379</v>
+        <v>381</v>
       </c>
       <c r="H86" s="16" t="s">
         <v>115</v>
       </c>
       <c r="I86" s="16" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="J86" s="16" t="s">
         <v>17</v>
@@ -4188,31 +4194,31 @@
     </row>
     <row r="87" spans="1:10">
       <c r="A87" s="28" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="B87" s="16" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="C87" s="17">
         <v>1</v>
       </c>
       <c r="D87" s="16" t="s">
-        <v>400</v>
+        <v>402</v>
       </c>
       <c r="E87" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F87" s="16" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="G87" s="16" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H87" s="16" t="s">
         <v>115</v>
       </c>
       <c r="I87" s="16" t="s">
-        <v>399</v>
+        <v>401</v>
       </c>
       <c r="J87" s="16" t="s">
         <v>17</v>
@@ -4220,31 +4226,31 @@
     </row>
     <row r="88" spans="1:10">
       <c r="A88" s="28" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="B88" s="16" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="C88" s="17">
         <v>1</v>
       </c>
       <c r="D88" s="16" t="s">
-        <v>402</v>
+        <v>404</v>
       </c>
       <c r="E88" s="16" t="s">
         <v>5</v>
       </c>
       <c r="F88" s="16" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="G88" s="16" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="H88" s="16" t="s">
         <v>115</v>
       </c>
       <c r="I88" s="16" t="s">
-        <v>401</v>
+        <v>403</v>
       </c>
       <c r="J88" s="16" t="s">
         <v>17</v>

</xml_diff>